<commit_message>
Include printing of the coefficients with the obj. Change to objective to scale by SD of the team variation in the trait Update the Calibration with the 1st iteration of results
</commit_message>
<xml_diff>
--- a/ExcelInputs/GEPEP_calibration.xlsx
+++ b/ExcelInputs/GEPEP_calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBE9164-C9A9-4DBA-B6BA-AC89FBD41A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F056F479-917E-4097-8B75-8616CC21B5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{08305449-70BC-467B-94A3-5CFFCBC3DBD2}"/>
+    <workbookView xWindow="3225" yWindow="450" windowWidth="25140" windowHeight="15075" activeTab="4" xr2:uid="{08305449-70BC-467B-94A3-5CFFCBC3DBD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Weights" sheetId="10" r:id="rId1"/>
@@ -564,7 +564,9 @@
   </sheetPr>
   <dimension ref="B1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -605,34 +607,34 @@
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>1</v>
+        <v>3.0966014953309635</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>1.413120046235661</v>
       </c>
       <c r="D2">
-        <v>0.25</v>
+        <v>6.4641864182834199E-2</v>
       </c>
       <c r="E2">
-        <v>0.25</v>
+        <v>3.0508130267892637E-2</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>29.015211341242807</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>7.9745703353327011</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>17.457801868409902</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0.40937577019250732</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>231.42038342001354</v>
       </c>
       <c r="K2">
-        <v>0.5</v>
+        <v>0.48837722660222549</v>
       </c>
     </row>
   </sheetData>
@@ -652,7 +654,7 @@
       <selection activeCell="A3" sqref="A3:XFD31"/>
       <selection pane="topRight" activeCell="A3" sqref="A3:XFD31"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD31"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +728,7 @@
       <c r="J2" s="1">
         <v>0.86</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2">
         <v>29</v>
       </c>
     </row>
@@ -746,7 +748,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,34 +796,34 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>4.08</v>
+        <v>3.8341017900000001</v>
       </c>
       <c r="C2">
-        <v>18</v>
+        <v>18.589628000000001</v>
       </c>
       <c r="D2">
-        <v>51</v>
+        <v>41.0079669</v>
       </c>
       <c r="E2">
-        <v>60000000</v>
+        <v>56392901.100000001</v>
       </c>
       <c r="F2">
-        <v>1.302</v>
+        <v>1.7229718199999999</v>
       </c>
       <c r="G2">
-        <v>7.9349999999999996</v>
+        <v>8.9106451700000004</v>
       </c>
       <c r="H2">
-        <v>1.7397800000000001</v>
+        <v>1.9655323600000001</v>
       </c>
       <c r="I2">
-        <v>58.880013793103451</v>
+        <v>58.8780614</v>
       </c>
       <c r="J2">
-        <v>8.219178082191781E-5</v>
+        <v>-1.6263011500000001E-4</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>1.2497876800000001</v>
       </c>
     </row>
   </sheetData>
@@ -837,7 +839,9 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:M2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -884,34 +888,34 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>3.08</v>
+        <v>2.8341017900000001</v>
       </c>
       <c r="C2">
-        <v>17</v>
+        <v>17.589628000000001</v>
       </c>
       <c r="D2">
-        <v>41</v>
+        <v>31.0079669</v>
       </c>
       <c r="E2">
-        <v>45000000</v>
+        <v>41392901.100000001</v>
       </c>
       <c r="F2">
-        <v>-2.698</v>
+        <v>-2.2770281800000003</v>
       </c>
       <c r="G2">
-        <v>6.9349999999999996</v>
+        <v>7.9106451700000004</v>
       </c>
       <c r="H2">
-        <v>0.7397800000000001</v>
+        <v>0.96553236000000009</v>
       </c>
       <c r="I2">
-        <v>53.880013793103451</v>
+        <v>53.8780614</v>
       </c>
       <c r="J2">
-        <v>-1.9178082191780824E-4</v>
+        <v>-4.3660271773972607E-4</v>
       </c>
       <c r="K2">
-        <v>0.75</v>
+        <v>0.99978768000000007</v>
       </c>
     </row>
   </sheetData>
@@ -926,7 +930,9 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:M2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -973,34 +979,34 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>5.08</v>
+        <v>4.8341017900000001</v>
       </c>
       <c r="C2">
-        <v>19</v>
+        <v>19.589628000000001</v>
       </c>
       <c r="D2">
-        <v>61</v>
+        <v>51.0079669</v>
       </c>
       <c r="E2">
-        <v>75000000</v>
+        <v>71392901.099999994</v>
       </c>
       <c r="F2">
-        <v>2.302</v>
+        <v>2.7229718199999997</v>
       </c>
       <c r="G2">
-        <v>8.9349999999999987</v>
+        <v>9.9106451700000004</v>
       </c>
       <c r="H2">
-        <v>5.7397799999999997</v>
+        <v>5.9655323600000001</v>
       </c>
       <c r="I2">
-        <v>63.880013793103451</v>
+        <v>63.8780614</v>
       </c>
       <c r="J2">
-        <v>2.1917808219178083E-4</v>
+        <v>-2.5643813630136977E-5</v>
       </c>
       <c r="K2">
-        <v>1.25</v>
+        <v>1.4997876800000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix naming for variables read into Sheep calibration. Handle different numbers of traits and coefficients Update team coefficients after first calibration attempt
</commit_message>
<xml_diff>
--- a/ExcelInputs/GEPEP_calibration.xlsx
+++ b/ExcelInputs/GEPEP_calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C985D259-22B3-4490-B7A5-91360077DE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DDA61D-A98B-4F69-893A-A1E9B89235B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{08305449-70BC-467B-94A3-5CFFCBC3DBD2}"/>
+    <workbookView xWindow="3150" yWindow="420" windowWidth="25140" windowHeight="15075" activeTab="4" xr2:uid="{08305449-70BC-467B-94A3-5CFFCBC3DBD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Weights" sheetId="10" r:id="rId1"/>
@@ -874,11 +874,11 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="A1:XFD1048576"/>
       <selection pane="topRight" activeCell="B3" sqref="A1:XFD1048576"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="A1:XFD1048576"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,37 +929,37 @@
         <v>6</v>
       </c>
       <c r="B2" s="2">
-        <v>3.7</v>
+        <v>3.7410000000000001</v>
       </c>
       <c r="C2" s="2">
-        <v>18.8</v>
+        <v>18.811</v>
       </c>
       <c r="D2" s="2">
-        <v>30</v>
+        <v>34.848999999999997</v>
       </c>
       <c r="E2" s="2">
-        <v>106</v>
+        <v>105.3</v>
       </c>
       <c r="F2" s="2">
-        <v>0.06</v>
+        <v>5.7799999999999997E-2</v>
       </c>
       <c r="G2" s="2">
-        <v>1.45</v>
+        <v>1.4810000000000001</v>
       </c>
       <c r="H2" s="2">
-        <v>0.76</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="I2" s="2">
-        <v>65</v>
+        <v>64.75</v>
       </c>
       <c r="J2" s="2">
-        <v>0.19109999999999999</v>
+        <v>0.42697000000000002</v>
       </c>
       <c r="K2" s="2">
-        <v>0.86</v>
+        <v>0.75109999999999999</v>
       </c>
       <c r="L2" s="2">
-        <v>29</v>
+        <v>27.73</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -967,37 +967,37 @@
         <v>20</v>
       </c>
       <c r="B3" s="4">
-        <v>4.1309759999999995</v>
+        <v>4.1767516799999997</v>
       </c>
       <c r="C3" s="3">
-        <v>23.079000000000001</v>
+        <v>23.09</v>
       </c>
       <c r="D3" s="3">
-        <v>33.459000000000003</v>
+        <v>38.308</v>
       </c>
       <c r="E3" s="3">
-        <v>120.23099999999999</v>
+        <v>119.53099999999999</v>
       </c>
       <c r="F3" s="6">
-        <v>3.6999999999999998E-2</v>
+        <v>3.4799999999999998E-2</v>
       </c>
       <c r="G3" s="3">
-        <v>1.5649999999999999</v>
+        <v>1.5960000000000001</v>
       </c>
       <c r="H3" s="3">
-        <v>0.79700000000000004</v>
+        <v>0.80100000000000005</v>
       </c>
       <c r="I3" s="3">
-        <v>69.298000000000002</v>
+        <v>69.048000000000002</v>
       </c>
       <c r="J3" s="5">
-        <v>0.20717576099179622</v>
+        <v>0.44306118809935435</v>
       </c>
       <c r="K3" s="3">
-        <v>0.85967326409</v>
+        <v>0.75077326409</v>
       </c>
       <c r="L3" s="3">
-        <v>30.684000000000001</v>
+        <v>29.414000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1005,37 +1005,37 @@
         <v>41</v>
       </c>
       <c r="B4" s="4">
-        <v>3.8961740000000002</v>
+        <v>3.9393478200000005</v>
       </c>
       <c r="C4" s="3">
-        <v>18.650000000000002</v>
+        <v>18.661000000000001</v>
       </c>
       <c r="D4" s="3">
-        <v>26.134999999999998</v>
+        <v>30.983999999999995</v>
       </c>
       <c r="E4" s="3">
-        <v>99.49</v>
+        <v>98.789999999999992</v>
       </c>
       <c r="F4" s="6">
-        <v>0.11199999999999999</v>
+        <v>0.10979999999999999</v>
       </c>
       <c r="G4" s="3">
-        <v>1.208</v>
+        <v>1.2390000000000001</v>
       </c>
       <c r="H4" s="3">
-        <v>0.753</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="I4" s="3">
-        <v>62.789000000000001</v>
+        <v>62.539000000000001</v>
       </c>
       <c r="J4" s="5">
-        <v>0.16651315243102088</v>
+        <v>0.41848976763793333</v>
       </c>
       <c r="K4" s="3">
-        <v>0.86023742049999996</v>
+        <v>0.75133742049999996</v>
       </c>
       <c r="L4" s="3">
-        <v>28.283999999999999</v>
+        <v>27.013999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1043,37 +1043,37 @@
         <v>27</v>
       </c>
       <c r="B5" s="4">
-        <v>3.6334</v>
+        <v>3.6736620000000002</v>
       </c>
       <c r="C5" s="3">
-        <v>17.824999999999999</v>
+        <v>17.835999999999999</v>
       </c>
       <c r="D5" s="3">
-        <v>24.172000000000001</v>
+        <v>29.020999999999997</v>
       </c>
       <c r="E5" s="3">
-        <v>107.45699999999999</v>
+        <v>106.75699999999999</v>
       </c>
       <c r="F5" s="6">
-        <v>0.06</v>
+        <v>5.7799999999999997E-2</v>
       </c>
       <c r="G5" s="3">
-        <v>1.532</v>
+        <v>1.5630000000000002</v>
       </c>
       <c r="H5" s="3">
-        <v>0.63900000000000001</v>
+        <v>0.64300000000000002</v>
       </c>
       <c r="I5" s="3">
-        <v>67.067000000000007</v>
+        <v>66.817000000000007</v>
       </c>
       <c r="J5" s="5">
-        <v>0.20134469038333472</v>
+        <v>0.42874988512882617</v>
       </c>
       <c r="K5" s="3">
-        <v>0.86331519999999995</v>
+        <v>0.75441519999999995</v>
       </c>
       <c r="L5" s="3">
-        <v>29.861000000000001</v>
+        <v>28.591000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1081,37 +1081,37 @@
         <v>37</v>
       </c>
       <c r="B6" s="4">
-        <v>3.8964699999999999</v>
+        <v>3.9396470999999997</v>
       </c>
       <c r="C6" s="3">
-        <v>16.93</v>
+        <v>16.940999999999999</v>
       </c>
       <c r="D6" s="3">
-        <v>20.439999999999998</v>
+        <v>25.288999999999994</v>
       </c>
       <c r="E6" s="3">
-        <v>87.652000000000001</v>
+        <v>86.951999999999998</v>
       </c>
       <c r="F6" s="6">
-        <v>4.1999999999999996E-2</v>
+        <v>3.9800000000000002E-2</v>
       </c>
       <c r="G6" s="3">
-        <v>1.4829999999999999</v>
+        <v>1.514</v>
       </c>
       <c r="H6" s="3">
-        <v>0.80900000000000005</v>
+        <v>0.81300000000000006</v>
       </c>
       <c r="I6" s="3">
-        <v>64.281000000000006</v>
+        <v>64.031000000000006</v>
       </c>
       <c r="J6" s="5">
-        <v>0.19126188586205517</v>
+        <v>0.42892719809843949</v>
       </c>
       <c r="K6" s="3">
-        <v>0.86167660000000001</v>
+        <v>0.75277660000000002</v>
       </c>
       <c r="L6" s="3">
-        <v>28.803000000000001</v>
+        <v>27.533000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1119,37 +1119,37 @@
         <v>28</v>
       </c>
       <c r="B7" s="4">
-        <v>2.9905620000000002</v>
+        <v>3.0237006599999998</v>
       </c>
       <c r="C7" s="3">
-        <v>16.817</v>
+        <v>16.827999999999999</v>
       </c>
       <c r="D7" s="3">
-        <v>28.097999999999999</v>
+        <v>32.946999999999996</v>
       </c>
       <c r="E7" s="3">
-        <v>100.80799999999999</v>
+        <v>100.108</v>
       </c>
       <c r="F7" s="6">
-        <v>4.4999999999999998E-2</v>
+        <v>4.2799999999999998E-2</v>
       </c>
       <c r="G7" s="3">
-        <v>1.6359999999999999</v>
+        <v>1.667</v>
       </c>
       <c r="H7" s="3">
-        <v>0.72</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="I7" s="3">
-        <v>64.622</v>
+        <v>64.372</v>
       </c>
       <c r="J7" s="5">
-        <v>0.19649782854097236</v>
+        <v>0.43434045374696995</v>
       </c>
       <c r="K7" s="3">
-        <v>0.86036988655000002</v>
+        <v>0.75146988655000002</v>
       </c>
       <c r="L7" s="3">
-        <v>28.608000000000001</v>
+        <v>27.338000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1157,37 +1157,37 @@
         <v>34</v>
       </c>
       <c r="B8" s="4">
-        <v>3.2194069999999999</v>
+        <v>3.2550815099999997</v>
       </c>
       <c r="C8" s="3">
-        <v>19.490000000000002</v>
+        <v>19.501000000000001</v>
       </c>
       <c r="D8" s="3">
-        <v>25.253</v>
+        <v>30.101999999999997</v>
       </c>
       <c r="E8" s="3">
-        <v>129.923</v>
+        <v>129.22299999999998</v>
       </c>
       <c r="F8" s="6">
-        <v>4.4999999999999998E-2</v>
+        <v>4.2799999999999998E-2</v>
       </c>
       <c r="G8" s="3">
-        <v>1.4339999999999999</v>
+        <v>1.4650000000000001</v>
       </c>
       <c r="H8" s="3">
-        <v>0.80200000000000005</v>
+        <v>0.80600000000000005</v>
       </c>
       <c r="I8" s="3">
-        <v>64.822999999999993</v>
+        <v>64.572999999999993</v>
       </c>
       <c r="J8" s="5">
-        <v>0.20133441888356132</v>
+        <v>0.44459029973808939</v>
       </c>
       <c r="K8" s="3">
-        <v>0.86373800000000001</v>
+        <v>0.75483800000000001</v>
       </c>
       <c r="L8" s="3">
-        <v>28.318000000000001</v>
+        <v>27.048000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1195,37 +1195,37 @@
         <v>18</v>
       </c>
       <c r="B9" s="4">
-        <v>3.9992929999999998</v>
+        <v>4.0436094899999997</v>
       </c>
       <c r="C9" s="3">
-        <v>18.003</v>
+        <v>18.013999999999999</v>
       </c>
       <c r="D9" s="3">
-        <v>28.414999999999999</v>
+        <v>33.263999999999996</v>
       </c>
       <c r="E9" s="3">
-        <v>104.78400000000001</v>
+        <v>104.084</v>
       </c>
       <c r="F9" s="6">
-        <v>5.1999999999999998E-2</v>
+        <v>4.9799999999999997E-2</v>
       </c>
       <c r="G9" s="3">
-        <v>1.39</v>
+        <v>1.421</v>
       </c>
       <c r="H9" s="3">
-        <v>0.85299999999999998</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="I9" s="3">
-        <v>65.709999999999994</v>
+        <v>65.459999999999994</v>
       </c>
       <c r="J9" s="5">
-        <v>0.18354673900752688</v>
+        <v>0.43705246585317437</v>
       </c>
       <c r="K9" s="3">
-        <v>0.85923404388000002</v>
+        <v>0.75033404388000002</v>
       </c>
       <c r="L9" s="3">
-        <v>29.4</v>
+        <v>28.13</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1233,37 +1233,37 @@
         <v>24</v>
       </c>
       <c r="B10" s="4">
-        <v>4.2569610000000004</v>
+        <v>4.3041327300000001</v>
       </c>
       <c r="C10" s="3">
-        <v>19.03</v>
+        <v>19.041</v>
       </c>
       <c r="D10" s="3">
-        <v>22.655000000000001</v>
+        <v>27.503999999999998</v>
       </c>
       <c r="E10" s="3">
-        <v>94.653000000000006</v>
+        <v>93.953000000000003</v>
       </c>
       <c r="F10" s="6">
-        <v>0.11199999999999999</v>
+        <v>0.10979999999999999</v>
       </c>
       <c r="G10" s="3">
-        <v>1.347</v>
+        <v>1.3780000000000001</v>
       </c>
       <c r="H10" s="3">
-        <v>0.75800000000000001</v>
+        <v>0.76200000000000001</v>
       </c>
       <c r="I10" s="3">
-        <v>67.492999999999995</v>
+        <v>67.242999999999995</v>
       </c>
       <c r="J10" s="5">
-        <v>0.18385070474464282</v>
+        <v>0.42981859770537534</v>
       </c>
       <c r="K10" s="3">
-        <v>0.85354770000000002</v>
+        <v>0.74464770000000002</v>
       </c>
       <c r="L10" s="3">
-        <v>29.547000000000001</v>
+        <v>28.277000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1271,37 +1271,37 @@
         <v>25</v>
       </c>
       <c r="B11" s="4">
-        <v>3.7442519999999999</v>
+        <v>3.78574236</v>
       </c>
       <c r="C11" s="3">
-        <v>19.859000000000002</v>
+        <v>19.87</v>
       </c>
       <c r="D11" s="3">
-        <v>36.889000000000003</v>
+        <v>41.738</v>
       </c>
       <c r="E11" s="3">
-        <v>118.10299999999999</v>
+        <v>117.40299999999999</v>
       </c>
       <c r="F11" s="6">
-        <v>3.8999999999999993E-2</v>
+        <v>3.6799999999999999E-2</v>
       </c>
       <c r="G11" s="3">
-        <v>1.363</v>
+        <v>1.3940000000000001</v>
       </c>
       <c r="H11" s="3">
-        <v>0.83099999999999996</v>
+        <v>0.83499999999999996</v>
       </c>
       <c r="I11" s="3">
-        <v>67.356999999999999</v>
+        <v>67.106999999999999</v>
       </c>
       <c r="J11" s="5">
-        <v>0.1766375074065771</v>
+        <v>0.41537153221951056</v>
       </c>
       <c r="K11" s="3">
-        <v>0.86525439999999998</v>
+        <v>0.75635439999999998</v>
       </c>
       <c r="L11" s="3">
-        <v>28.675999999999998</v>
+        <v>27.405999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1309,37 +1309,37 @@
         <v>30</v>
       </c>
       <c r="B12" s="4">
-        <v>3.0815820000000005</v>
+        <v>3.1157292600000002</v>
       </c>
       <c r="C12" s="3">
-        <v>17.693999999999999</v>
+        <v>17.704999999999998</v>
       </c>
       <c r="D12" s="3">
-        <v>30.382999999999999</v>
+        <v>35.231999999999999</v>
       </c>
       <c r="E12" s="3">
-        <v>109.592</v>
+        <v>108.892</v>
       </c>
       <c r="F12" s="6">
-        <v>4.5999999999999999E-2</v>
+        <v>4.3799999999999999E-2</v>
       </c>
       <c r="G12" s="3">
-        <v>1.304</v>
+        <v>1.3350000000000002</v>
       </c>
       <c r="H12" s="3">
-        <v>0.84899999999999998</v>
+        <v>0.85299999999999998</v>
       </c>
       <c r="I12" s="3">
-        <v>62.981999999999999</v>
+        <v>62.731999999999999</v>
       </c>
       <c r="J12" s="5">
-        <v>0.22329874752548756</v>
+        <v>0.44758570685255628</v>
       </c>
       <c r="K12" s="3">
-        <v>0.85995556574800003</v>
+        <v>0.75105556574800003</v>
       </c>
       <c r="L12" s="3">
-        <v>29.206</v>
+        <v>27.936</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1347,37 +1347,37 @@
         <v>21</v>
       </c>
       <c r="B13" s="4">
-        <v>4.0837640000000004</v>
+        <v>4.1290165200000004</v>
       </c>
       <c r="C13" s="3">
-        <v>19.102</v>
+        <v>19.113</v>
       </c>
       <c r="D13" s="3">
-        <v>31.626999999999999</v>
+        <v>36.475999999999999</v>
       </c>
       <c r="E13" s="3">
-        <v>96.122</v>
+        <v>95.421999999999997</v>
       </c>
       <c r="F13" s="6">
-        <v>7.4999999999999997E-2</v>
+        <v>7.2800000000000004E-2</v>
       </c>
       <c r="G13" s="3">
-        <v>1.448</v>
+        <v>1.4790000000000001</v>
       </c>
       <c r="H13" s="3">
-        <v>0.73099999999999998</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="I13" s="3">
-        <v>66.828999999999994</v>
+        <v>66.578999999999994</v>
       </c>
       <c r="J13" s="5">
-        <v>0.17777352681930988</v>
+        <v>0.43427466077942428</v>
       </c>
       <c r="K13" s="3">
-        <v>0.85912012161999995</v>
+        <v>0.75022012161999996</v>
       </c>
       <c r="L13" s="3">
-        <v>27.753</v>
+        <v>26.483000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1385,37 +1385,37 @@
         <v>43</v>
       </c>
       <c r="B14" s="4">
-        <v>3.3387320000000003</v>
+        <v>3.3757287600000003</v>
       </c>
       <c r="C14" s="3">
-        <v>20.344999999999999</v>
+        <v>20.356000000000002</v>
       </c>
       <c r="D14" s="3">
-        <v>30.98</v>
+        <v>35.828999999999994</v>
       </c>
       <c r="E14" s="3">
-        <v>123.61799999999999</v>
+        <v>122.91799999999999</v>
       </c>
       <c r="F14" s="6">
-        <v>0.106</v>
+        <v>0.1038</v>
       </c>
       <c r="G14" s="3">
-        <v>1.4359999999999999</v>
+        <v>1.4670000000000001</v>
       </c>
       <c r="H14" s="3">
-        <v>0.73299999999999998</v>
+        <v>0.73699999999999999</v>
       </c>
       <c r="I14" s="3">
-        <v>62.055</v>
+        <v>61.805</v>
       </c>
       <c r="J14" s="5">
-        <v>0.21032973981461439</v>
+        <v>0.45351982770159682</v>
       </c>
       <c r="K14" s="3">
-        <v>0.86302349999999994</v>
+        <v>0.75412349999999995</v>
       </c>
       <c r="L14" s="3">
-        <v>29.495000000000001</v>
+        <v>28.225000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1423,37 +1423,37 @@
         <v>39</v>
       </c>
       <c r="B15" s="4">
-        <v>3.658042</v>
+        <v>3.6985770599999999</v>
       </c>
       <c r="C15" s="3">
-        <v>18.926000000000002</v>
+        <v>18.937000000000001</v>
       </c>
       <c r="D15" s="3">
-        <v>34.374000000000002</v>
+        <v>39.222999999999999</v>
       </c>
       <c r="E15" s="3">
-        <v>94.762</v>
+        <v>94.061999999999998</v>
       </c>
       <c r="F15" s="6">
-        <v>9.2999999999999999E-2</v>
+        <v>9.0799999999999992E-2</v>
       </c>
       <c r="G15" s="3">
-        <v>1.4949999999999999</v>
+        <v>1.526</v>
       </c>
       <c r="H15" s="3">
-        <v>0.71299999999999997</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="I15" s="3">
-        <v>68.450999999999993</v>
+        <v>68.200999999999993</v>
       </c>
       <c r="J15" s="5">
-        <v>0.17537216508733486</v>
+        <v>0.4378074198964898</v>
       </c>
       <c r="K15" s="3">
-        <v>0.86070075310999994</v>
+        <v>0.75180075310999994</v>
       </c>
       <c r="L15" s="3">
-        <v>30.582999999999998</v>
+        <v>29.312999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1461,37 +1461,37 @@
         <v>31</v>
       </c>
       <c r="B16" s="4">
-        <v>3.6348060000000002</v>
+        <v>3.6750835800000003</v>
       </c>
       <c r="C16" s="3">
-        <v>18.058</v>
+        <v>18.068999999999999</v>
       </c>
       <c r="D16" s="3">
-        <v>34.073</v>
+        <v>38.921999999999997</v>
       </c>
       <c r="E16" s="3">
-        <v>109.24</v>
+        <v>108.53999999999999</v>
       </c>
       <c r="F16" s="6">
-        <v>3.2000000000000001E-2</v>
+        <v>2.9799999999999997E-2</v>
       </c>
       <c r="G16" s="3">
-        <v>1.5149999999999999</v>
+        <v>1.546</v>
       </c>
       <c r="H16" s="3">
-        <v>0.70199999999999996</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="I16" s="3">
-        <v>61.987000000000002</v>
+        <v>61.737000000000002</v>
       </c>
       <c r="J16" s="5">
-        <v>0.20818691527891905</v>
+        <v>0.45490976228296698</v>
       </c>
       <c r="K16" s="3">
-        <v>0.84854200000000002</v>
+        <v>0.73964200000000002</v>
       </c>
       <c r="L16" s="3">
-        <v>26.962</v>
+        <v>25.692</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1499,37 +1499,37 @@
         <v>26</v>
       </c>
       <c r="B17" s="4">
-        <v>3.9550780000000003</v>
+        <v>3.9989045400000003</v>
       </c>
       <c r="C17" s="3">
-        <v>18.922000000000001</v>
+        <v>18.933</v>
       </c>
       <c r="D17" s="3">
-        <v>30.972000000000001</v>
+        <v>35.820999999999998</v>
       </c>
       <c r="E17" s="3">
-        <v>99.644999999999996</v>
+        <v>98.944999999999993</v>
       </c>
       <c r="F17" s="6">
-        <v>5.2999999999999999E-2</v>
+        <v>5.0799999999999998E-2</v>
       </c>
       <c r="G17" s="3">
-        <v>1.452</v>
+        <v>1.4830000000000001</v>
       </c>
       <c r="H17" s="3">
-        <v>0.79500000000000004</v>
+        <v>0.79900000000000004</v>
       </c>
       <c r="I17" s="3">
-        <v>62.543999999999997</v>
+        <v>62.293999999999997</v>
       </c>
       <c r="J17" s="5">
-        <v>0.20916427779429331</v>
+        <v>0.47298946718481838</v>
       </c>
       <c r="K17" s="3">
-        <v>0.86251440000000001</v>
+        <v>0.75361440000000002</v>
       </c>
       <c r="L17" s="3">
-        <v>29.082999999999998</v>
+        <v>27.812999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1537,37 +1537,37 @@
         <v>35</v>
       </c>
       <c r="B18" s="4">
-        <v>4.0225660000000003</v>
+        <v>4.0671403800000006</v>
       </c>
       <c r="C18" s="3">
-        <v>18.393000000000001</v>
+        <v>18.404</v>
       </c>
       <c r="D18" s="3">
-        <v>25.404</v>
+        <v>30.252999999999997</v>
       </c>
       <c r="E18" s="3">
-        <v>102.25</v>
+        <v>101.55</v>
       </c>
       <c r="F18" s="6">
-        <v>8.3999999999999991E-2</v>
+        <v>8.1799999999999998E-2</v>
       </c>
       <c r="G18" s="3">
-        <v>1.2909999999999999</v>
+        <v>1.3220000000000001</v>
       </c>
       <c r="H18" s="3">
-        <v>0.748</v>
+        <v>0.752</v>
       </c>
       <c r="I18" s="3">
-        <v>62.887</v>
+        <v>62.637</v>
       </c>
       <c r="J18" s="5">
-        <v>0.17984099994381852</v>
+        <v>0.46174589423619505</v>
       </c>
       <c r="K18" s="3">
-        <v>0.86050191573000001</v>
+        <v>0.75160191573000001</v>
       </c>
       <c r="L18" s="3">
-        <v>30.245000000000001</v>
+        <v>28.975000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1575,37 +1575,37 @@
         <v>36</v>
       </c>
       <c r="B19" s="4">
-        <v>3.062157</v>
+        <v>3.09608901</v>
       </c>
       <c r="C19" s="3">
-        <v>17.929000000000002</v>
+        <v>17.940000000000001</v>
       </c>
       <c r="D19" s="3">
-        <v>27.856999999999999</v>
+        <v>32.705999999999996</v>
       </c>
       <c r="E19" s="3">
-        <v>102.452</v>
+        <v>101.752</v>
       </c>
       <c r="F19" s="6">
-        <v>2.4999999999999994E-2</v>
+        <v>2.2799999999999994E-2</v>
       </c>
       <c r="G19" s="3">
-        <v>1.63</v>
+        <v>1.661</v>
       </c>
       <c r="H19" s="3">
-        <v>0.71199999999999997</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="I19" s="3">
-        <v>66.741</v>
+        <v>66.491</v>
       </c>
       <c r="J19" s="5">
-        <v>0.18078031591255619</v>
+        <v>0.45144163725630937</v>
       </c>
       <c r="K19" s="3">
-        <v>0.86172989999999994</v>
+        <v>0.75282989999999994</v>
       </c>
       <c r="L19" s="3">
-        <v>28.137</v>
+        <v>26.867000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1613,37 +1613,37 @@
         <v>32</v>
       </c>
       <c r="B20" s="4">
-        <v>3.7140600000000004</v>
+        <v>3.7552158000000002</v>
       </c>
       <c r="C20" s="3">
-        <v>19.571000000000002</v>
+        <v>19.582000000000001</v>
       </c>
       <c r="D20" s="3">
-        <v>30.026</v>
+        <v>34.875</v>
       </c>
       <c r="E20" s="3">
-        <v>103.32299999999999</v>
+        <v>102.62299999999999</v>
       </c>
       <c r="F20" s="6">
-        <v>6.5000000000000002E-2</v>
+        <v>6.2799999999999995E-2</v>
       </c>
       <c r="G20" s="3">
-        <v>1.427</v>
+        <v>1.4580000000000002</v>
       </c>
       <c r="H20" s="3">
-        <v>0.753</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="I20" s="3">
-        <v>68.718000000000004</v>
+        <v>68.468000000000004</v>
       </c>
       <c r="J20" s="5">
-        <v>0.19870822339220931</v>
+        <v>0.4590652877560768</v>
       </c>
       <c r="K20" s="3">
-        <v>0.85820160000000001</v>
+        <v>0.74930160000000001</v>
       </c>
       <c r="L20" s="3">
-        <v>29.940999999999999</v>
+        <v>28.670999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1651,37 +1651,37 @@
         <v>22</v>
       </c>
       <c r="B21" s="4">
-        <v>3.8608020000000005</v>
+        <v>3.9035838600000003</v>
       </c>
       <c r="C21" s="3">
-        <v>18.185000000000002</v>
+        <v>18.196000000000002</v>
       </c>
       <c r="D21" s="3">
-        <v>29.137</v>
+        <v>33.985999999999997</v>
       </c>
       <c r="E21" s="3">
-        <v>97.89</v>
+        <v>97.19</v>
       </c>
       <c r="F21" s="6">
-        <v>5.1999999999999998E-2</v>
+        <v>4.9799999999999997E-2</v>
       </c>
       <c r="G21" s="3">
-        <v>1.4689999999999999</v>
+        <v>1.5</v>
       </c>
       <c r="H21" s="3">
-        <v>0.74399999999999999</v>
+        <v>0.748</v>
       </c>
       <c r="I21" s="3">
-        <v>67.721999999999994</v>
+        <v>67.471999999999994</v>
       </c>
       <c r="J21" s="5">
-        <v>0.20434987783865849</v>
+        <v>0.47233059270229338</v>
       </c>
       <c r="K21" s="3">
-        <v>0.85917387307000004</v>
+        <v>0.75027387307000004</v>
       </c>
       <c r="L21" s="3">
-        <v>30.795000000000002</v>
+        <v>29.524999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1689,37 +1689,37 @@
         <v>19</v>
       </c>
       <c r="B22" s="4">
-        <v>3.9766490000000001</v>
+        <v>4.02071457</v>
       </c>
       <c r="C22" s="3">
-        <v>17.874000000000002</v>
+        <v>17.885000000000002</v>
       </c>
       <c r="D22" s="3">
-        <v>29.167000000000002</v>
+        <v>34.015999999999998</v>
       </c>
       <c r="E22" s="3">
-        <v>110.07599999999999</v>
+        <v>109.37599999999999</v>
       </c>
       <c r="F22" s="6">
-        <v>3.3000000000000002E-2</v>
+        <v>3.0799999999999998E-2</v>
       </c>
       <c r="G22" s="3">
-        <v>1.246</v>
+        <v>1.2770000000000001</v>
       </c>
       <c r="H22" s="3">
-        <v>0.84299999999999997</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="I22" s="3">
-        <v>63.435000000000002</v>
+        <v>63.185000000000002</v>
       </c>
       <c r="J22" s="5">
-        <v>0.1811126962170955</v>
+        <v>0.462358716026947</v>
       </c>
       <c r="K22" s="3">
-        <v>0.8542381</v>
+        <v>0.7453381</v>
       </c>
       <c r="L22" s="3">
-        <v>27.884</v>
+        <v>26.614000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1727,37 +1727,37 @@
         <v>44</v>
       </c>
       <c r="B23" s="4">
-        <v>4.1065560000000003</v>
+        <v>4.1520610800000002</v>
       </c>
       <c r="C23" s="3">
-        <v>19.022000000000002</v>
+        <v>19.033000000000001</v>
       </c>
       <c r="D23" s="3">
-        <v>33.619</v>
+        <v>38.467999999999996</v>
       </c>
       <c r="E23" s="3">
-        <v>103.976</v>
+        <v>103.276</v>
       </c>
       <c r="F23" s="6">
-        <v>4.9999999999999975E-3</v>
+        <v>2.7999999999999969E-3</v>
       </c>
       <c r="G23" s="3">
-        <v>1.3220000000000001</v>
+        <v>1.3530000000000002</v>
       </c>
       <c r="H23" s="3">
-        <v>0.65700000000000003</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="I23" s="3">
-        <v>62.113</v>
+        <v>61.863</v>
       </c>
       <c r="J23" s="5">
-        <v>0.20897759486519993</v>
+        <v>0.48025173799970505</v>
       </c>
       <c r="K23" s="3">
-        <v>0.85289530000000002</v>
+        <v>0.74399530000000003</v>
       </c>
       <c r="L23" s="3">
-        <v>28.097000000000001</v>
+        <v>26.827000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1765,37 +1765,37 @@
         <v>29</v>
       </c>
       <c r="B24" s="4">
-        <v>3.4382619999999999</v>
+        <v>3.4763616599999998</v>
       </c>
       <c r="C24" s="3">
-        <v>18.201000000000001</v>
+        <v>18.212</v>
       </c>
       <c r="D24" s="3">
-        <v>40.085000000000001</v>
+        <v>44.933999999999997</v>
       </c>
       <c r="E24" s="3">
-        <v>108.437</v>
+        <v>107.73699999999999</v>
       </c>
       <c r="F24" s="6">
-        <v>4.1999999999999996E-2</v>
+        <v>3.9800000000000002E-2</v>
       </c>
       <c r="G24" s="3">
-        <v>1.4869999999999999</v>
+        <v>1.518</v>
       </c>
       <c r="H24" s="3">
-        <v>0.73799999999999999</v>
+        <v>0.74199999999999999</v>
       </c>
       <c r="I24" s="3">
-        <v>66.564999999999998</v>
+        <v>66.314999999999998</v>
       </c>
       <c r="J24" s="5">
-        <v>0.2021740806318168</v>
+        <v>0.49134124573908</v>
       </c>
       <c r="K24" s="3">
-        <v>0.86541139999999994</v>
+        <v>0.75651139999999995</v>
       </c>
       <c r="L24" s="3">
-        <v>29.506</v>
+        <v>28.236000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1803,37 +1803,37 @@
         <v>40</v>
       </c>
       <c r="B25" s="4">
-        <v>3.4964260000000005</v>
+        <v>3.5351701800000002</v>
       </c>
       <c r="C25" s="3">
-        <v>19.824999999999999</v>
+        <v>19.835999999999999</v>
       </c>
       <c r="D25" s="3">
-        <v>34.143000000000001</v>
+        <v>38.991999999999997</v>
       </c>
       <c r="E25" s="3">
-        <v>108.52200000000001</v>
+        <v>107.822</v>
       </c>
       <c r="F25" s="6">
-        <v>6.3E-2</v>
+        <v>6.08E-2</v>
       </c>
       <c r="G25" s="3">
-        <v>1.3579999999999999</v>
+        <v>1.389</v>
       </c>
       <c r="H25" s="3">
-        <v>0.79</v>
+        <v>0.79400000000000004</v>
       </c>
       <c r="I25" s="3">
-        <v>68.614000000000004</v>
+        <v>68.364000000000004</v>
       </c>
       <c r="J25" s="5">
-        <v>0.17329727833583053</v>
+        <v>0.47355395118246868</v>
       </c>
       <c r="K25" s="3">
-        <v>0.86075600448</v>
+        <v>0.75185600448000001</v>
       </c>
       <c r="L25" s="3">
-        <v>30.623999999999999</v>
+        <v>29.353999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1841,37 +1841,37 @@
         <v>33</v>
       </c>
       <c r="B26" s="4">
-        <v>3.3136830000000002</v>
+        <v>3.3504021900000001</v>
       </c>
       <c r="C26" s="3">
-        <v>18.646000000000001</v>
+        <v>18.657</v>
       </c>
       <c r="D26" s="3">
-        <v>25.462</v>
+        <v>30.310999999999996</v>
       </c>
       <c r="E26" s="3">
-        <v>121.843</v>
+        <v>121.143</v>
       </c>
       <c r="F26" s="6">
-        <v>0.11799999999999999</v>
+        <v>0.1158</v>
       </c>
       <c r="G26" s="3">
-        <v>1.55</v>
+        <v>1.5810000000000002</v>
       </c>
       <c r="H26" s="3">
-        <v>0.80100000000000005</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="I26" s="3">
-        <v>63.942</v>
+        <v>63.692</v>
       </c>
       <c r="J26" s="5">
-        <v>0.19523232984616015</v>
+        <v>0.47770170813618695</v>
       </c>
       <c r="K26" s="3">
-        <v>0.86626340000000002</v>
+        <v>0.75736340000000002</v>
       </c>
       <c r="L26" s="3">
-        <v>28.492000000000001</v>
+        <v>27.222000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1879,37 +1879,37 @@
         <v>42</v>
       </c>
       <c r="B27" s="4">
-        <v>3.9797200000000008</v>
+        <v>4.0238196000000004</v>
       </c>
       <c r="C27" s="3">
-        <v>19.164000000000001</v>
+        <v>19.175000000000001</v>
       </c>
       <c r="D27" s="3">
-        <v>33.965000000000003</v>
+        <v>38.813999999999993</v>
       </c>
       <c r="E27" s="3">
-        <v>108.069</v>
+        <v>107.369</v>
       </c>
       <c r="F27" s="6">
-        <v>4.8000000000000001E-2</v>
+        <v>4.5799999999999993E-2</v>
       </c>
       <c r="G27" s="3">
-        <v>1.5859999999999999</v>
+        <v>1.617</v>
       </c>
       <c r="H27" s="3">
-        <v>0.70199999999999996</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="I27" s="3">
-        <v>63.524999999999999</v>
+        <v>63.274999999999999</v>
       </c>
       <c r="J27" s="5">
-        <v>0.17490840809428312</v>
+        <v>0.4615255433380282</v>
       </c>
       <c r="K27" s="3">
-        <v>0.85987838213000001</v>
+        <v>0.75097838213000001</v>
       </c>
       <c r="L27" s="3">
-        <v>27.768000000000001</v>
+        <v>26.498000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1917,37 +1917,37 @@
         <v>38</v>
       </c>
       <c r="B28" s="4">
-        <v>3.7424390000000005</v>
+        <v>3.7839092700000005</v>
       </c>
       <c r="C28" s="3">
-        <v>18.309000000000001</v>
+        <v>18.32</v>
       </c>
       <c r="D28" s="3">
-        <v>31.041</v>
+        <v>35.889999999999993</v>
       </c>
       <c r="E28" s="3">
-        <v>97.432999999999993</v>
+        <v>96.733000000000004</v>
       </c>
       <c r="F28" s="6">
-        <v>0.14000000000000001</v>
+        <v>0.13780000000000001</v>
       </c>
       <c r="G28" s="3">
-        <v>1.323</v>
+        <v>1.3540000000000001</v>
       </c>
       <c r="H28" s="3">
-        <v>0.80900000000000005</v>
+        <v>0.81300000000000006</v>
       </c>
       <c r="I28" s="3">
-        <v>63.149000000000001</v>
+        <v>62.899000000000001</v>
       </c>
       <c r="J28" s="5">
-        <v>0.19834505547699571</v>
+        <v>0.46878602592258201</v>
       </c>
       <c r="K28" s="3">
-        <v>0.86286770000000002</v>
+        <v>0.75396770000000002</v>
       </c>
       <c r="L28" s="3">
-        <v>28.393999999999998</v>
+        <v>27.123999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1955,37 +1955,37 @@
         <v>23</v>
       </c>
       <c r="B29" s="4">
-        <v>3.5265439999999999</v>
+        <v>3.5656219199999999</v>
       </c>
       <c r="C29" s="3">
-        <v>19.027000000000001</v>
+        <v>19.038</v>
       </c>
       <c r="D29" s="3">
-        <v>33.025999999999996</v>
+        <v>37.875</v>
       </c>
       <c r="E29" s="3">
-        <v>109.419</v>
+        <v>108.71899999999999</v>
       </c>
       <c r="F29" s="6">
-        <v>1.1999999999999997E-2</v>
+        <v>9.7999999999999962E-3</v>
       </c>
       <c r="G29" s="3">
-        <v>1.645</v>
+        <v>1.6760000000000002</v>
       </c>
       <c r="H29" s="3">
-        <v>0.83599999999999997</v>
+        <v>0.84</v>
       </c>
       <c r="I29" s="3">
-        <v>64.566999999999993</v>
+        <v>64.316999999999993</v>
       </c>
       <c r="J29" s="5">
-        <v>0.17410906380552105</v>
+        <v>0.4518105168356612</v>
       </c>
       <c r="K29" s="3">
-        <v>0.85872369999999998</v>
+        <v>0.74982369999999998</v>
       </c>
       <c r="L29" s="3">
-        <v>28.824000000000002</v>
+        <v>27.554000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1993,37 +1993,37 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>3.8459279999999998</v>
+        <v>3.8885450399999999</v>
       </c>
       <c r="C30" s="3">
-        <v>19.129000000000001</v>
+        <v>19.14</v>
       </c>
       <c r="D30" s="3">
-        <v>30.106999999999999</v>
+        <v>34.955999999999996</v>
       </c>
       <c r="E30" s="3">
-        <v>94.926000000000002</v>
+        <v>94.225999999999999</v>
       </c>
       <c r="F30" s="6">
-        <v>0.06</v>
+        <v>5.7799999999999997E-2</v>
       </c>
       <c r="G30" s="3">
-        <v>1.3859999999999999</v>
+        <v>1.417</v>
       </c>
       <c r="H30" s="3">
-        <v>0.77100000000000002</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="I30" s="3">
-        <v>61.889000000000003</v>
+        <v>61.639000000000003</v>
       </c>
       <c r="J30" s="5">
-        <v>0.16972152454056619</v>
+        <v>0.43044746848378551</v>
       </c>
       <c r="K30" s="3">
-        <v>0.86166719999999997</v>
+        <v>0.75276719999999997</v>
       </c>
       <c r="L30" s="3">
-        <v>28.51</v>
+        <v>27.240000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2031,37 +2031,37 @@
         <v>16</v>
       </c>
       <c r="B31" s="4">
-        <v>3.6946720000000002</v>
+        <v>3.7356129600000001</v>
       </c>
       <c r="C31" s="3">
-        <v>19.193000000000001</v>
+        <v>19.204000000000001</v>
       </c>
       <c r="D31" s="3">
-        <v>29.036000000000001</v>
+        <v>33.884999999999998</v>
       </c>
       <c r="E31" s="3">
-        <v>109.30500000000001</v>
+        <v>108.605</v>
       </c>
       <c r="F31" s="6">
-        <v>4.2999999999999997E-2</v>
+        <v>4.0799999999999996E-2</v>
       </c>
       <c r="G31" s="3">
-        <v>1.74</v>
+        <v>1.7710000000000001</v>
       </c>
       <c r="H31" s="3">
-        <v>0.67400000000000004</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="I31" s="3">
-        <v>62.846000000000004</v>
+        <v>62.596000000000004</v>
       </c>
       <c r="J31" s="5">
-        <v>0.18760710440865561</v>
+        <v>0.42696999999999924</v>
       </c>
       <c r="K31" s="3">
-        <v>0.85495100000000002</v>
+        <v>0.74605100000000002</v>
       </c>
       <c r="L31" s="3">
-        <v>28.521000000000001</v>
+        <v>27.251000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2076,12 +2076,12 @@
   </sheetPr>
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="A1:XFD1048576"/>
       <selection pane="topRight" activeCell="B3" sqref="A1:XFD1048576"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="A1:XFD1048576"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,10 +2166,10 @@
         <v>27</v>
       </c>
       <c r="L2" s="1">
-        <v>0</v>
+        <v>8.219178082191781E-5</v>
       </c>
       <c r="M2" s="1">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2180,13 +2180,13 @@
         <v>4.3096127999999991</v>
       </c>
       <c r="C3" s="2">
-        <v>22.833478723404255</v>
+        <v>22.831003136462709</v>
       </c>
       <c r="D3" s="2">
-        <v>44.723530000000011</v>
+        <v>44.080197423168535</v>
       </c>
       <c r="E3" s="3">
-        <v>50253262.46974574</v>
+        <v>50213752.081050105</v>
       </c>
       <c r="F3">
         <v>1.7229718199999999</v>
@@ -2204,13 +2204,13 @@
         <v>0.04</v>
       </c>
       <c r="K3" s="4">
-        <v>28.607576099179621</v>
+        <v>28.609118809935435</v>
       </c>
       <c r="L3" s="3">
-        <v>0</v>
+        <v>8.2227550617654902E-5</v>
       </c>
       <c r="M3">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2221,13 +2221,13 @@
         <v>4.0646572000000001</v>
       </c>
       <c r="C4" s="2">
-        <v>18.451595744680855</v>
+        <v>18.451682526181493</v>
       </c>
       <c r="D4" s="2">
-        <v>34.933783333333331</v>
+        <v>35.652627048121893</v>
       </c>
       <c r="E4" s="3">
-        <v>60729721.580058306</v>
+        <v>60756149.407834806</v>
       </c>
       <c r="F4">
         <v>1.7229718199999999</v>
@@ -2245,13 +2245,13 @@
         <v>0.04</v>
       </c>
       <c r="K4" s="4">
-        <v>24.54131524310209</v>
+        <v>26.151976763793332</v>
       </c>
       <c r="L4" s="3">
-        <v>0</v>
+        <v>8.2165808451626916E-5</v>
       </c>
       <c r="M4">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2262,13 +2262,13 @@
         <v>3.7905199999999999</v>
       </c>
       <c r="C5" s="2">
-        <v>17.635372340425533</v>
+        <v>17.635936420179682</v>
       </c>
       <c r="D5" s="2">
-        <v>32.309906666666663</v>
+        <v>33.393844873597523</v>
       </c>
       <c r="E5" s="3">
-        <v>56227142.019598536</v>
+        <v>56222074.430716492</v>
       </c>
       <c r="F5">
         <v>1.7229718199999999</v>
@@ -2286,13 +2286,13 @@
         <v>0.04</v>
       </c>
       <c r="K5" s="4">
-        <v>28.024469038333471</v>
+        <v>27.177988512882614</v>
       </c>
       <c r="L5" s="3">
-        <v>0</v>
+        <v>8.1830597495043141E-5</v>
       </c>
       <c r="M5">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2303,13 +2303,13 @@
         <v>4.0649659999999992</v>
       </c>
       <c r="C6" s="2">
-        <v>16.749893617021275</v>
+        <v>16.750975493062569</v>
       </c>
       <c r="D6" s="2">
-        <v>27.321466666666662</v>
+        <v>29.099512181124279</v>
       </c>
       <c r="E6" s="3">
-        <v>68931684.388262674</v>
+        <v>69027739.442451</v>
       </c>
       <c r="F6">
         <v>1.7229718199999999</v>
@@ -2327,13 +2327,13 @@
         <v>0.04</v>
       </c>
       <c r="K6" s="4">
-        <v>27.016188586205519</v>
+        <v>27.195719809843947</v>
       </c>
       <c r="L6" s="3">
-        <v>0</v>
+        <v>8.2008721545465769E-5</v>
       </c>
       <c r="M6">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2344,13 +2344,13 @@
         <v>3.1198835999999996</v>
       </c>
       <c r="C7" s="2">
-        <v>16.63809574468085</v>
+        <v>16.639242996119293</v>
       </c>
       <c r="D7" s="2">
-        <v>37.557659999999998</v>
+        <v>37.911409222646277</v>
       </c>
       <c r="E7" s="3">
-        <v>59935719.387350217</v>
+        <v>59956247.252966784</v>
       </c>
       <c r="F7">
         <v>1.7229718199999999</v>
@@ -2368,13 +2368,13 @@
         <v>0.04</v>
       </c>
       <c r="K7" s="4">
-        <v>27.539782854097236</v>
+        <v>27.737045374696994</v>
       </c>
       <c r="L7" s="3">
-        <v>0</v>
+        <v>8.2151324597668887E-5</v>
       </c>
       <c r="M7">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2385,13 +2385,13 @@
         <v>3.3586245999999997</v>
       </c>
       <c r="C8" s="2">
-        <v>19.282659574468088</v>
+        <v>19.282260379565152</v>
       </c>
       <c r="D8" s="2">
-        <v>33.754843333333334</v>
+        <v>34.637728485752817</v>
       </c>
       <c r="E8" s="3">
-        <v>46504468.031064555</v>
+        <v>46447613.814878158</v>
       </c>
       <c r="F8">
         <v>1.7229718199999999</v>
@@ -2409,13 +2409,13 @@
         <v>0.04</v>
       </c>
       <c r="K8" s="4">
-        <v>28.023441888356132</v>
+        <v>28.762029973808936</v>
       </c>
       <c r="L8" s="3">
-        <v>0</v>
+        <v>8.1784762525657771E-5</v>
       </c>
       <c r="M8">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2426,13 +2426,13 @@
         <v>4.1722353999999999</v>
       </c>
       <c r="C9" s="2">
-        <v>17.811478723404257</v>
+        <v>17.811939822444316</v>
       </c>
       <c r="D9" s="2">
-        <v>37.981383333333333</v>
+        <v>38.276174352205231</v>
       </c>
       <c r="E9" s="3">
-        <v>57661475.034356393</v>
+        <v>57665923.677030079</v>
       </c>
       <c r="F9">
         <v>1.7229718199999999</v>
@@ -2450,13 +2450,13 @@
         <v>0.04</v>
       </c>
       <c r="K9" s="4">
-        <v>26.244673900752687</v>
+        <v>28.008246585317433</v>
       </c>
       <c r="L9" s="3">
-        <v>0</v>
+        <v>8.2275683848906573E-5</v>
       </c>
       <c r="M9">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2467,13 +2467,13 @@
         <v>4.4410458000000004</v>
       </c>
       <c r="C10" s="2">
-        <v>18.827553191489365</v>
+        <v>18.827420126521716</v>
       </c>
       <c r="D10" s="2">
-        <v>30.282183333333332</v>
+        <v>31.648265373468394</v>
       </c>
       <c r="E10" s="3">
-        <v>63833159.012392625</v>
+        <v>63884069.694421679</v>
       </c>
       <c r="F10">
         <v>1.7229718199999999</v>
@@ -2491,13 +2491,13 @@
         <v>0.04</v>
       </c>
       <c r="K10" s="4">
-        <v>26.275070474464282</v>
+        <v>27.284859770537533</v>
       </c>
       <c r="L10" s="3">
-        <v>0</v>
+        <v>8.2903964620239157E-5</v>
       </c>
       <c r="M10">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2508,13 +2508,13 @@
         <v>3.9061655999999996</v>
       </c>
       <c r="C11" s="2">
-        <v>19.647734042553196</v>
+        <v>19.647121365158686</v>
       </c>
       <c r="D11" s="2">
-        <v>49.308296666666671</v>
+        <v>48.027025165714946</v>
       </c>
       <c r="E11" s="3">
-        <v>51158734.32512299</v>
+        <v>51123906.544125788</v>
       </c>
       <c r="F11">
         <v>1.7229718199999999</v>
@@ -2532,13 +2532,13 @@
         <v>0.04</v>
       </c>
       <c r="K11" s="4">
-        <v>25.553750740657712</v>
+        <v>25.840153221951056</v>
       </c>
       <c r="L11" s="3">
-        <v>0</v>
+        <v>8.1620793870363511E-5</v>
       </c>
       <c r="M11">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2549,13 +2549,13 @@
         <v>3.2148395999999999</v>
       </c>
       <c r="C12" s="2">
-        <v>17.505765957446808</v>
+        <v>17.506405826378181</v>
       </c>
       <c r="D12" s="2">
-        <v>40.611943333333329</v>
+        <v>40.540709919940312</v>
       </c>
       <c r="E12" s="3">
-        <v>55131761.442441054</v>
+        <v>55119751.680564225</v>
       </c>
       <c r="F12">
         <v>1.7229718199999999</v>
@@ -2573,13 +2573,13 @@
         <v>0.04</v>
       </c>
       <c r="K12" s="4">
-        <v>30.219874752548758</v>
+        <v>29.061570685255624</v>
       </c>
       <c r="L12" s="3">
-        <v>0</v>
+        <v>8.2196643485171937E-5</v>
       </c>
       <c r="M12">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2590,13 +2590,13 @@
         <v>4.2603591999999999</v>
       </c>
       <c r="C13" s="2">
-        <v>18.898787234042555</v>
+        <v>18.898612513954603</v>
       </c>
       <c r="D13" s="2">
-        <v>42.274756666666669</v>
+        <v>41.972154150764737</v>
       </c>
       <c r="E13" s="3">
-        <v>62857618.443228394</v>
+        <v>62900588.962713003</v>
       </c>
       <c r="F13">
         <v>1.7229718199999999</v>
@@ -2614,13 +2614,13 @@
         <v>0.04</v>
       </c>
       <c r="K13" s="4">
-        <v>25.667352681930989</v>
+        <v>27.730466077942427</v>
       </c>
       <c r="L13" s="3">
-        <v>0</v>
+        <v>8.2288177557855458E-5</v>
       </c>
       <c r="M13">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2631,13 +2631,13 @@
         <v>3.4831096000000001</v>
       </c>
       <c r="C14" s="2">
-        <v>20.128563829787236</v>
+        <v>20.127669980330658</v>
       </c>
       <c r="D14" s="2">
-        <v>41.409933333333335</v>
+        <v>41.227665069298979</v>
       </c>
       <c r="E14" s="3">
-        <v>48876377.226617485</v>
+        <v>48830114.385199897</v>
       </c>
       <c r="F14">
         <v>1.7229718199999999</v>
@@ -2655,13 +2655,13 @@
         <v>0.04</v>
       </c>
       <c r="K14" s="4">
-        <v>28.922973981461439</v>
+        <v>29.65498277015968</v>
       </c>
       <c r="L14" s="3">
-        <v>0</v>
+        <v>8.1862250115985604E-5</v>
       </c>
       <c r="M14">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2672,13 +2672,13 @@
         <v>3.8162275999999999</v>
       </c>
       <c r="C15" s="2">
-        <v>18.724659574468085</v>
+        <v>18.724586678007551</v>
       </c>
       <c r="D15" s="2">
-        <v>45.946580000000004</v>
+        <v>45.13306838072829</v>
       </c>
       <c r="E15" s="3">
-        <v>63759734.914839275</v>
+        <v>63810040.186260127</v>
       </c>
       <c r="F15">
         <v>1.7229718199999999</v>
@@ -2696,13 +2696,13 @@
         <v>0.04</v>
       </c>
       <c r="K15" s="4">
-        <v>25.427216508733487</v>
+        <v>28.083741989648978</v>
       </c>
       <c r="L15" s="3">
-        <v>0</v>
+        <v>8.2115169903680327E-5</v>
       </c>
       <c r="M15">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2713,13 +2713,13 @@
         <v>3.7919868000000001</v>
       </c>
       <c r="C16" s="2">
-        <v>17.865893617021278</v>
+        <v>17.866322896177767</v>
       </c>
       <c r="D16" s="2">
-        <v>45.544243333333334</v>
+        <v>44.786714109443601</v>
       </c>
       <c r="E16" s="3">
-        <v>55309410.472354449</v>
+        <v>55298507.462686568</v>
       </c>
       <c r="F16">
         <v>1.7229718199999999</v>
@@ -2737,13 +2737,13 @@
         <v>0.04</v>
       </c>
       <c r="K16" s="4">
-        <v>28.708691527891908</v>
+        <v>29.793976228296696</v>
       </c>
       <c r="L16" s="3">
-        <v>0</v>
+        <v>8.3465036565449861E-5</v>
       </c>
       <c r="M16">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -2754,13 +2754,13 @@
         <v>4.1261083999999997</v>
       </c>
       <c r="C17" s="2">
-        <v>18.720702127659575</v>
+        <v>18.720631545372392</v>
       </c>
       <c r="D17" s="2">
-        <v>41.399239999999999</v>
+        <v>41.218459640161846</v>
       </c>
       <c r="E17" s="3">
-        <v>60635255.155803107</v>
+        <v>60660973.267977163</v>
       </c>
       <c r="F17">
         <v>1.7229718199999999</v>
@@ -2778,13 +2778,13 @@
         <v>0.04</v>
       </c>
       <c r="K17" s="4">
-        <v>28.806427779429331</v>
+        <v>31.601946718481837</v>
       </c>
       <c r="L17" s="3">
-        <v>0</v>
+        <v>8.1917551701961197E-5</v>
       </c>
       <c r="M17">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -2795,13 +2795,13 @@
         <v>4.1965148000000001</v>
       </c>
       <c r="C18" s="2">
-        <v>18.197329787234043</v>
+        <v>18.197565254372442</v>
       </c>
       <c r="D18" s="2">
-        <v>33.956679999999999</v>
+        <v>34.811480960716231</v>
       </c>
       <c r="E18" s="3">
-        <v>59090464.547677256</v>
+        <v>59104874.446085669</v>
       </c>
       <c r="F18">
         <v>1.7229718199999999</v>
@@ -2819,13 +2819,13 @@
         <v>0.04</v>
       </c>
       <c r="K18" s="4">
-        <v>25.874099994381854</v>
+        <v>30.477589423619506</v>
       </c>
       <c r="L18" s="3">
-        <v>0</v>
+        <v>8.2136893591313603E-5</v>
       </c>
       <c r="M18">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2836,13 +2836,13 @@
         <v>3.1945745999999997</v>
       </c>
       <c r="C19" s="2">
-        <v>17.73826595744681</v>
+        <v>17.738769868693851</v>
       </c>
       <c r="D19" s="2">
-        <v>37.235523333333333</v>
+        <v>37.634095669890101</v>
       </c>
       <c r="E19" s="3">
-        <v>58973958.536680587</v>
+        <v>58987538.328484945</v>
       </c>
       <c r="F19">
         <v>1.7229718199999999</v>
@@ -2860,13 +2860,13 @@
         <v>0.04</v>
       </c>
       <c r="K19" s="4">
-        <v>25.96803159125562</v>
+        <v>29.447163725630936</v>
       </c>
       <c r="L19" s="3">
-        <v>0</v>
+        <v>8.200291536686105E-5</v>
       </c>
       <c r="M19">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2877,13 +2877,13 @@
         <v>3.8746679999999998</v>
       </c>
       <c r="C20" s="2">
-        <v>19.362797872340426</v>
+        <v>19.362351815427147</v>
       </c>
       <c r="D20" s="2">
-        <v>40.134753333333329</v>
+        <v>40.129917644695688</v>
       </c>
       <c r="E20" s="3">
-        <v>58476815.423477843</v>
+        <v>58486888.904046856</v>
       </c>
       <c r="F20">
         <v>1.7229718199999999</v>
@@ -2901,13 +2901,13 @@
         <v>0.04</v>
       </c>
       <c r="K20" s="4">
-        <v>27.760822339220933</v>
+        <v>30.20952877560768</v>
       </c>
       <c r="L20" s="3">
-        <v>0</v>
+        <v>8.2389049449971109E-5</v>
       </c>
       <c r="M20">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -2918,13 +2918,13 @@
         <v>4.0277555999999999</v>
       </c>
       <c r="C21" s="2">
-        <v>17.99154255319149</v>
+        <v>17.991898357344112</v>
       </c>
       <c r="D21" s="2">
-        <v>38.94645666666667</v>
+        <v>39.10696433183162</v>
       </c>
       <c r="E21" s="3">
-        <v>61722341.403616309</v>
+        <v>61756353.53431423</v>
       </c>
       <c r="F21">
         <v>1.7229718199999999</v>
@@ -2942,13 +2942,13 @@
         <v>0.04</v>
       </c>
       <c r="K21" s="4">
-        <v>28.324987783865851</v>
+        <v>31.536059270229337</v>
       </c>
       <c r="L21" s="3">
-        <v>0</v>
+        <v>8.2282282232134591E-5</v>
       </c>
       <c r="M21">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2959,13 +2959,13 @@
         <v>4.1486121999999996</v>
       </c>
       <c r="C22" s="2">
-        <v>17.683851063829788</v>
+        <v>17.6843867949604</v>
       </c>
       <c r="D22" s="2">
-        <v>38.986556666666672</v>
+        <v>39.141484691095869</v>
       </c>
       <c r="E22" s="3">
-        <v>54889349.176932305</v>
+        <v>54875841.135166764</v>
       </c>
       <c r="F22">
         <v>1.7229718199999999</v>
@@ -2983,13 +2983,13 @@
         <v>0.04</v>
       </c>
       <c r="K22" s="4">
-        <v>26.00126962170955</v>
+        <v>30.538871602694698</v>
       </c>
       <c r="L22" s="3">
-        <v>0</v>
+        <v>8.2827171421053701E-5</v>
       </c>
       <c r="M22">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -3000,13 +3000,13 @@
         <v>4.2841367999999997</v>
       </c>
       <c r="C23" s="2">
-        <v>18.819638297872341</v>
+        <v>18.819509861251397</v>
       </c>
       <c r="D23" s="2">
-        <v>44.937396666666672</v>
+        <v>44.264306005911223</v>
       </c>
       <c r="E23" s="3">
-        <v>58109563.745479733</v>
+        <v>58117084.317750491</v>
       </c>
       <c r="F23">
         <v>1.7229718199999999</v>
@@ -3024,13 +3024,13 @@
         <v>0.04</v>
       </c>
       <c r="K23" s="4">
-        <v>28.787759486519995</v>
+        <v>32.3281737999705</v>
       </c>
       <c r="L23" s="3">
-        <v>0</v>
+        <v>8.2976662050610365E-5</v>
       </c>
       <c r="M23">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -3041,13 +3041,13 @@
         <v>3.5869435999999997</v>
       </c>
       <c r="C24" s="2">
-        <v>18.007372340425533</v>
+        <v>18.007718887884749</v>
       </c>
       <c r="D24" s="2">
-        <v>53.580283333333341</v>
+        <v>51.704594106000179</v>
       </c>
       <c r="E24" s="3">
-        <v>55718988.906000718</v>
+        <v>55710665.787983701</v>
       </c>
       <c r="F24">
         <v>1.7229718199999999</v>
@@ -3065,13 +3065,13 @@
         <v>0.04</v>
       </c>
       <c r="K24" s="4">
-        <v>28.10740806318168</v>
+        <v>33.437124573908001</v>
       </c>
       <c r="L24" s="3">
-        <v>0</v>
+        <v>8.1603854978712121E-5</v>
       </c>
       <c r="M24">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -3082,13 +3082,13 @@
         <v>3.6476228000000002</v>
       </c>
       <c r="C25" s="2">
-        <v>19.614095744680849</v>
+        <v>19.61350273775982</v>
       </c>
       <c r="D25" s="2">
-        <v>45.637810000000009</v>
+        <v>44.867261614393534</v>
       </c>
       <c r="E25" s="3">
-        <v>55675346.934262179</v>
+        <v>55666747.046057388</v>
       </c>
       <c r="F25">
         <v>1.7229718199999999</v>
@@ -3106,13 +3106,13 @@
         <v>0.04</v>
       </c>
       <c r="K25" s="4">
-        <v>25.219727833583054</v>
+        <v>31.658395118246865</v>
       </c>
       <c r="L25" s="3">
-        <v>0</v>
+        <v>8.2109135535918503E-5</v>
       </c>
       <c r="M25">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -3123,13 +3123,13 @@
         <v>3.4569774</v>
       </c>
       <c r="C26" s="2">
-        <v>18.447638297872341</v>
+        <v>18.44772739354633</v>
       </c>
       <c r="D26" s="2">
-        <v>34.03420666666667</v>
+        <v>34.878220321960455</v>
       </c>
       <c r="E26" s="3">
-        <v>49588404.750375479</v>
+        <v>49545578.366063245</v>
       </c>
       <c r="F26">
         <v>1.7229718199999999</v>
@@ -3147,13 +3147,13 @@
         <v>0.04</v>
       </c>
       <c r="K26" s="4">
-        <v>27.413232984616016</v>
+        <v>32.073170813618695</v>
       </c>
       <c r="L26" s="3">
-        <v>0</v>
+        <v>8.1512054286413189E-5</v>
       </c>
       <c r="M26">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -3164,13 +3164,13 @@
         <v>4.1518160000000002</v>
       </c>
       <c r="C27" s="2">
-        <v>18.960127659574468</v>
+        <v>18.959917069799591</v>
       </c>
       <c r="D27" s="2">
-        <v>45.399883333333342</v>
+        <v>44.662440816092278</v>
       </c>
       <c r="E27" s="3">
-        <v>55908724.981261969</v>
+        <v>55901610.334454075</v>
       </c>
       <c r="F27">
         <v>1.7229718199999999</v>
@@ -3188,13 +3188,13 @@
         <v>0.04</v>
       </c>
       <c r="K27" s="4">
-        <v>25.380840809428314</v>
+        <v>30.455554333802819</v>
       </c>
       <c r="L27" s="3">
-        <v>0</v>
+        <v>8.2205091443838385E-5</v>
       </c>
       <c r="M27">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -3205,13 +3205,13 @@
         <v>3.9042742000000001</v>
       </c>
       <c r="C28" s="2">
-        <v>18.11422340425532</v>
+        <v>18.114507469034077</v>
       </c>
       <c r="D28" s="2">
-        <v>41.49147</v>
+        <v>41.297856466469625</v>
       </c>
       <c r="E28" s="3">
-        <v>62011844.03641478</v>
+        <v>62048111.812928371</v>
       </c>
       <c r="F28">
         <v>1.7229718199999999</v>
@@ -3229,13 +3229,13 @@
         <v>0.04</v>
       </c>
       <c r="K28" s="4">
-        <v>27.724505547699572</v>
+        <v>31.181602592258198</v>
       </c>
       <c r="L28" s="3">
-        <v>0</v>
+        <v>8.1879166143778402E-5</v>
       </c>
       <c r="M28">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -3246,13 +3246,13 @@
         <v>3.6790431999999997</v>
       </c>
       <c r="C29" s="2">
-        <v>18.82458510638298</v>
+        <v>18.824453777045349</v>
       </c>
       <c r="D29" s="2">
-        <v>44.144753333333327</v>
+        <v>43.581953571121126</v>
       </c>
       <c r="E29" s="3">
-        <v>55218929.070819512</v>
+        <v>55207461.43728327</v>
       </c>
       <c r="F29">
         <v>1.7229718199999999</v>
@@ -3270,13 +3270,13 @@
         <v>0.04</v>
       </c>
       <c r="K29" s="4">
-        <v>25.300906380552107</v>
+        <v>29.484051683566118</v>
       </c>
       <c r="L29" s="3">
-        <v>0</v>
+        <v>8.2331682201219392E-5</v>
       </c>
       <c r="M29">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -3287,13 +3287,13 @@
         <v>4.0122383999999993</v>
       </c>
       <c r="C30" s="2">
-        <v>18.925500000000003</v>
+        <v>18.925309659241936</v>
       </c>
       <c r="D30" s="2">
-        <v>40.243023333333333</v>
+        <v>40.223122614709169</v>
       </c>
       <c r="E30" s="3">
-        <v>63649579.672587067</v>
+        <v>63698979.050368257</v>
       </c>
       <c r="F30">
         <v>1.7229718199999999</v>
@@ -3311,13 +3311,13 @@
         <v>0.04</v>
       </c>
       <c r="K30" s="4">
-        <v>24.86215245405662</v>
+        <v>27.347746848378549</v>
       </c>
       <c r="L30" s="3">
-        <v>0</v>
+        <v>8.2009745609721663E-5</v>
       </c>
       <c r="M30">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -3328,13 +3328,13 @@
         <v>3.8544415999999999</v>
       </c>
       <c r="C31" s="2">
-        <v>18.988819148936173</v>
+        <v>18.988591781404498</v>
       </c>
       <c r="D31" s="2">
-        <v>38.81145333333334</v>
+        <v>38.990745788975296</v>
       </c>
       <c r="E31" s="3">
-        <v>55276519.829833947</v>
+        <v>55265411.353068456</v>
       </c>
       <c r="F31">
         <v>1.7229718199999999</v>
@@ -3352,13 +3352,13 @@
         <v>0.04</v>
       </c>
       <c r="K31" s="4">
-        <v>26.650710440865563</v>
+        <v>26.999999999999922</v>
       </c>
       <c r="L31" s="3">
-        <v>0</v>
+        <v>8.2748024699842853E-5</v>
       </c>
       <c r="M31">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3375,7 +3375,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:XFD1048576"/>
+      <selection activeCell="B2" sqref="B2:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3459,10 +3459,10 @@
         <v>22</v>
       </c>
       <c r="L2">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9178082191780824E-4</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3473,13 +3473,13 @@
         <v>3.3096127999999991</v>
       </c>
       <c r="C3">
-        <v>21.833478723404255</v>
+        <v>21.831003136462709</v>
       </c>
       <c r="D3">
-        <v>29.723530000000011</v>
+        <v>29.080197423168535</v>
       </c>
       <c r="E3">
-        <v>35253262.46974574</v>
+        <v>35213752.081050105</v>
       </c>
       <c r="F3">
         <v>-2.2770281800000003</v>
@@ -3497,13 +3497,13 @@
         <v>0.02</v>
       </c>
       <c r="K3">
-        <v>23.607576099179621</v>
+        <v>23.609118809935435</v>
       </c>
       <c r="L3">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9174505212207115E-4</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -3514,13 +3514,13 @@
         <v>3.0646572000000001</v>
       </c>
       <c r="C4">
-        <v>17.451595744680855</v>
+        <v>17.451682526181493</v>
       </c>
       <c r="D4">
-        <v>19.933783333333331</v>
+        <v>20.652627048121893</v>
       </c>
       <c r="E4">
-        <v>45729721.580058306</v>
+        <v>45756149.407834806</v>
       </c>
       <c r="F4">
         <v>-2.2770281800000003</v>
@@ -3538,13 +3538,13 @@
         <v>0.02</v>
       </c>
       <c r="K4">
-        <v>19.54131524310209</v>
+        <v>21.151976763793332</v>
       </c>
       <c r="L4">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9180679428809915E-4</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3555,13 +3555,13 @@
         <v>2.7905199999999999</v>
       </c>
       <c r="C5">
-        <v>16.635372340425533</v>
+        <v>16.635936420179682</v>
       </c>
       <c r="D5">
-        <v>17.309906666666663</v>
+        <v>18.393844873597523</v>
       </c>
       <c r="E5">
-        <v>41227142.019598536</v>
+        <v>41222074.430716492</v>
       </c>
       <c r="F5">
         <v>-2.2770281800000003</v>
@@ -3579,13 +3579,13 @@
         <v>0.02</v>
       </c>
       <c r="K5">
-        <v>23.024469038333471</v>
+        <v>22.177988512882614</v>
       </c>
       <c r="L5">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9214200524468291E-4</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -3596,13 +3596,13 @@
         <v>3.0649659999999992</v>
       </c>
       <c r="C6">
-        <v>15.749893617021275</v>
+        <v>15.750975493062569</v>
       </c>
       <c r="D6">
-        <v>12.321466666666662</v>
+        <v>14.099512181124279</v>
       </c>
       <c r="E6">
-        <v>53931684.388262674</v>
+        <v>54027739.442451</v>
       </c>
       <c r="F6">
         <v>-2.2770281800000003</v>
@@ -3620,13 +3620,13 @@
         <v>0.02</v>
       </c>
       <c r="K6">
-        <v>22.016188586205519</v>
+        <v>22.195719809843947</v>
       </c>
       <c r="L6">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9196388119426029E-4</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3637,13 +3637,13 @@
         <v>2.1198835999999996</v>
       </c>
       <c r="C7">
-        <v>15.63809574468085</v>
+        <v>15.639242996119293</v>
       </c>
       <c r="D7">
-        <v>22.557659999999998</v>
+        <v>22.911409222646277</v>
       </c>
       <c r="E7">
-        <v>44935719.387350217</v>
+        <v>44956247.252966784</v>
       </c>
       <c r="F7">
         <v>-2.2770281800000003</v>
@@ -3661,13 +3661,13 @@
         <v>0.02</v>
       </c>
       <c r="K7">
-        <v>22.539782854097236</v>
+        <v>22.737045374696994</v>
       </c>
       <c r="L7">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9182127814205719E-4</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -3678,13 +3678,13 @@
         <v>2.3586245999999997</v>
       </c>
       <c r="C8">
-        <v>18.282659574468088</v>
+        <v>18.282260379565152</v>
       </c>
       <c r="D8">
-        <v>18.754843333333334</v>
+        <v>19.637728485752817</v>
       </c>
       <c r="E8">
-        <v>31504468.031064555</v>
+        <v>31447613.814878158</v>
       </c>
       <c r="F8">
         <v>-2.2770281800000003</v>
@@ -3702,13 +3702,13 @@
         <v>0.02</v>
       </c>
       <c r="K8">
-        <v>23.023441888356132</v>
+        <v>23.762029973808936</v>
       </c>
       <c r="L8">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9218784021406829E-4</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -3719,13 +3719,13 @@
         <v>3.1722353999999999</v>
       </c>
       <c r="C9">
-        <v>16.811478723404257</v>
+        <v>16.811939822444316</v>
       </c>
       <c r="D9">
-        <v>22.981383333333333</v>
+        <v>23.276174352205231</v>
       </c>
       <c r="E9">
-        <v>42661475.034356393</v>
+        <v>42665923.677030079</v>
       </c>
       <c r="F9">
         <v>-2.2770281800000003</v>
@@ -3743,13 +3743,13 @@
         <v>0.02</v>
       </c>
       <c r="K9">
-        <v>21.244673900752687</v>
+        <v>23.008246585317433</v>
       </c>
       <c r="L9">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9169691889081949E-4</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -3760,13 +3760,13 @@
         <v>3.4410458000000004</v>
       </c>
       <c r="C10">
-        <v>17.827553191489365</v>
+        <v>17.827420126521716</v>
       </c>
       <c r="D10">
-        <v>15.282183333333332</v>
+        <v>16.648265373468394</v>
       </c>
       <c r="E10">
-        <v>48833159.012392625</v>
+        <v>48884069.694421679</v>
       </c>
       <c r="F10">
         <v>-2.2770281800000003</v>
@@ -3784,13 +3784,13 @@
         <v>0.02</v>
       </c>
       <c r="K10">
-        <v>21.275070474464282</v>
+        <v>22.284859770537533</v>
       </c>
       <c r="L10">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9106863811948691E-4</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -3801,13 +3801,13 @@
         <v>2.9061655999999996</v>
       </c>
       <c r="C11">
-        <v>18.647734042553196</v>
+        <v>18.647121365158686</v>
       </c>
       <c r="D11">
-        <v>34.308296666666671</v>
+        <v>33.027025165714946</v>
       </c>
       <c r="E11">
-        <v>36158734.32512299</v>
+        <v>36123906.544125788</v>
       </c>
       <c r="F11">
         <v>-2.2770281800000003</v>
@@ -3825,13 +3825,13 @@
         <v>0.02</v>
       </c>
       <c r="K11">
-        <v>20.553750740657712</v>
+        <v>20.840153221951056</v>
       </c>
       <c r="L11">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9235180886936255E-4</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -3842,13 +3842,13 @@
         <v>2.2148395999999999</v>
       </c>
       <c r="C12">
-        <v>16.505765957446808</v>
+        <v>16.506405826378181</v>
       </c>
       <c r="D12">
-        <v>25.611943333333329</v>
+        <v>25.540709919940312</v>
       </c>
       <c r="E12">
-        <v>40131761.442441054</v>
+        <v>40119751.680564225</v>
       </c>
       <c r="F12">
         <v>-2.2770281800000003</v>
@@ -3866,13 +3866,13 @@
         <v>0.02</v>
       </c>
       <c r="K12">
-        <v>25.219874752548758</v>
+        <v>24.061570685255624</v>
       </c>
       <c r="L12">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9177595925455414E-4</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -3883,13 +3883,13 @@
         <v>3.2603591999999999</v>
       </c>
       <c r="C13">
-        <v>17.898787234042555</v>
+        <v>17.898612513954603</v>
       </c>
       <c r="D13">
-        <v>27.274756666666669</v>
+        <v>26.972154150764737</v>
       </c>
       <c r="E13">
-        <v>47857618.443228394</v>
+        <v>47900588.962713003</v>
       </c>
       <c r="F13">
         <v>-2.2770281800000003</v>
@@ -3907,13 +3907,13 @@
         <v>0.02</v>
       </c>
       <c r="K13">
-        <v>20.667352681930989</v>
+        <v>22.730466077942427</v>
       </c>
       <c r="L13">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.916844251818706E-4</v>
       </c>
       <c r="M13">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -3924,13 +3924,13 @@
         <v>2.4831096000000001</v>
       </c>
       <c r="C14">
-        <v>19.128563829787236</v>
+        <v>19.127669980330658</v>
       </c>
       <c r="D14">
-        <v>26.409933333333335</v>
+        <v>26.227665069298979</v>
       </c>
       <c r="E14">
-        <v>33876377.226617485</v>
+        <v>33830114.385199897</v>
       </c>
       <c r="F14">
         <v>-2.2770281800000003</v>
@@ -3948,13 +3948,13 @@
         <v>0.02</v>
       </c>
       <c r="K14">
-        <v>23.922973981461439</v>
+        <v>24.65498277015968</v>
       </c>
       <c r="L14">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9211035262374046E-4</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -3965,13 +3965,13 @@
         <v>2.8162275999999999</v>
       </c>
       <c r="C15">
-        <v>17.724659574468085</v>
+        <v>17.724586678007551</v>
       </c>
       <c r="D15">
-        <v>30.946580000000004</v>
+        <v>30.13306838072829</v>
       </c>
       <c r="E15">
-        <v>48759734.914839275</v>
+        <v>48810040.186260127</v>
       </c>
       <c r="F15">
         <v>-2.2770281800000003</v>
@@ -3989,13 +3989,13 @@
         <v>0.02</v>
       </c>
       <c r="K15">
-        <v>20.427216508733487</v>
+        <v>23.083741989648978</v>
       </c>
       <c r="L15">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9185743283604574E-4</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -4006,13 +4006,13 @@
         <v>2.7919868000000001</v>
       </c>
       <c r="C16">
-        <v>16.865893617021278</v>
+        <v>16.866322896177767</v>
       </c>
       <c r="D16">
-        <v>30.544243333333334</v>
+        <v>29.786714109443601</v>
       </c>
       <c r="E16">
-        <v>40309410.472354449</v>
+        <v>40298507.462686568</v>
       </c>
       <c r="F16">
         <v>-2.2770281800000003</v>
@@ -4030,13 +4030,13 @@
         <v>0.02</v>
       </c>
       <c r="K16">
-        <v>23.708691527891908</v>
+        <v>24.793976228296696</v>
       </c>
       <c r="L16">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9050756617427621E-4</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -4047,13 +4047,13 @@
         <v>3.1261083999999997</v>
       </c>
       <c r="C17">
-        <v>17.720702127659575</v>
+        <v>17.720631545372392</v>
       </c>
       <c r="D17">
-        <v>26.399239999999999</v>
+        <v>26.218459640161846</v>
       </c>
       <c r="E17">
-        <v>45635255.155803107</v>
+        <v>45660973.267977163</v>
       </c>
       <c r="F17">
         <v>-2.2770281800000003</v>
@@ -4071,13 +4071,13 @@
         <v>0.02</v>
       </c>
       <c r="K17">
-        <v>23.806427779429331</v>
+        <v>26.601946718481837</v>
       </c>
       <c r="L17">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9205505103776487E-4</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -4088,13 +4088,13 @@
         <v>3.1965148000000001</v>
       </c>
       <c r="C18">
-        <v>17.197329787234043</v>
+        <v>17.197565254372442</v>
       </c>
       <c r="D18">
-        <v>18.956679999999999</v>
+        <v>19.811480960716231</v>
       </c>
       <c r="E18">
-        <v>44090464.547677256</v>
+        <v>44104874.446085669</v>
       </c>
       <c r="F18">
         <v>-2.2770281800000003</v>
@@ -4112,13 +4112,13 @@
         <v>0.02</v>
       </c>
       <c r="K18">
-        <v>20.874099994381854</v>
+        <v>25.477589423619506</v>
       </c>
       <c r="L18">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9183570914841247E-4</v>
       </c>
       <c r="M18">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -4129,13 +4129,13 @@
         <v>2.1945745999999997</v>
       </c>
       <c r="C19">
-        <v>16.73826595744681</v>
+        <v>16.738769868693851</v>
       </c>
       <c r="D19">
-        <v>22.235523333333333</v>
+        <v>22.634095669890101</v>
       </c>
       <c r="E19">
-        <v>43973958.536680587</v>
+        <v>43987538.328484945</v>
       </c>
       <c r="F19">
         <v>-2.2770281800000003</v>
@@ -4153,13 +4153,13 @@
         <v>0.02</v>
       </c>
       <c r="K19">
-        <v>20.96803159125562</v>
+        <v>24.447163725630936</v>
       </c>
       <c r="L19">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9196968737286501E-4</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -4170,13 +4170,13 @@
         <v>2.8746679999999998</v>
       </c>
       <c r="C20">
-        <v>18.362797872340426</v>
+        <v>18.362351815427147</v>
       </c>
       <c r="D20">
-        <v>25.134753333333329</v>
+        <v>25.129917644695688</v>
       </c>
       <c r="E20">
-        <v>43476815.423477843</v>
+        <v>43486888.904046856</v>
       </c>
       <c r="F20">
         <v>-2.2770281800000003</v>
@@ -4194,13 +4194,13 @@
         <v>0.02</v>
       </c>
       <c r="K20">
-        <v>22.760822339220933</v>
+        <v>25.20952877560768</v>
       </c>
       <c r="L20">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9158355328975494E-4</v>
       </c>
       <c r="M20">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -4211,13 +4211,13 @@
         <v>3.0277555999999999</v>
       </c>
       <c r="C21">
-        <v>16.99154255319149</v>
+        <v>16.991898357344112</v>
       </c>
       <c r="D21">
-        <v>23.94645666666667</v>
+        <v>24.10696433183162</v>
       </c>
       <c r="E21">
-        <v>46722341.403616309</v>
+        <v>46756353.53431423</v>
       </c>
       <c r="F21">
         <v>-2.2770281800000003</v>
@@ -4235,13 +4235,13 @@
         <v>0.02</v>
       </c>
       <c r="K21">
-        <v>23.324987783865851</v>
+        <v>26.536059270229337</v>
       </c>
       <c r="L21">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9169032050759147E-4</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -4252,13 +4252,13 @@
         <v>3.1486121999999996</v>
       </c>
       <c r="C22">
-        <v>16.683851063829788</v>
+        <v>16.6843867949604</v>
       </c>
       <c r="D22">
-        <v>23.986556666666672</v>
+        <v>24.141484691095869</v>
       </c>
       <c r="E22">
-        <v>39889349.176932305</v>
+        <v>39875841.135166764</v>
       </c>
       <c r="F22">
         <v>-2.2770281800000003</v>
@@ -4276,13 +4276,13 @@
         <v>0.02</v>
       </c>
       <c r="K22">
-        <v>21.00126962170955</v>
+        <v>25.538871602694698</v>
       </c>
       <c r="L22">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9114543131867236E-4</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -4293,13 +4293,13 @@
         <v>3.2841367999999997</v>
       </c>
       <c r="C23">
-        <v>17.819638297872341</v>
+        <v>17.819509861251397</v>
       </c>
       <c r="D23">
-        <v>29.937396666666672</v>
+        <v>29.264306005911223</v>
       </c>
       <c r="E23">
-        <v>43109563.745479733</v>
+        <v>43117084.317750491</v>
       </c>
       <c r="F23">
         <v>-2.2770281800000003</v>
@@ -4317,13 +4317,13 @@
         <v>0.02</v>
       </c>
       <c r="K23">
-        <v>23.787759486519995</v>
+        <v>27.3281737999705</v>
       </c>
       <c r="L23">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.909959406891157E-4</v>
       </c>
       <c r="M23">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -4334,13 +4334,13 @@
         <v>2.5869435999999997</v>
       </c>
       <c r="C24">
-        <v>17.007372340425533</v>
+        <v>17.007718887884749</v>
       </c>
       <c r="D24">
-        <v>38.580283333333341</v>
+        <v>36.704594106000179</v>
       </c>
       <c r="E24">
-        <v>40718988.906000718</v>
+        <v>40710665.787983701</v>
       </c>
       <c r="F24">
         <v>-2.2770281800000003</v>
@@ -4358,13 +4358,13 @@
         <v>0.02</v>
       </c>
       <c r="K24">
-        <v>23.10740806318168</v>
+        <v>28.437124573908001</v>
       </c>
       <c r="L24">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9236874776101394E-4</v>
       </c>
       <c r="M24">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -4375,13 +4375,13 @@
         <v>2.6476228000000002</v>
       </c>
       <c r="C25">
-        <v>18.614095744680849</v>
+        <v>18.61350273775982</v>
       </c>
       <c r="D25">
-        <v>30.637810000000009</v>
+        <v>29.867261614393534</v>
       </c>
       <c r="E25">
-        <v>40675346.934262179</v>
+        <v>40666747.046057388</v>
       </c>
       <c r="F25">
         <v>-2.2770281800000003</v>
@@ -4399,13 +4399,13 @@
         <v>0.02</v>
       </c>
       <c r="K25">
-        <v>20.219727833583054</v>
+        <v>26.658395118246865</v>
       </c>
       <c r="L25">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9186346720380756E-4</v>
       </c>
       <c r="M25">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -4416,13 +4416,13 @@
         <v>2.4569774</v>
       </c>
       <c r="C26">
-        <v>17.447638297872341</v>
+        <v>17.44772739354633</v>
       </c>
       <c r="D26">
-        <v>19.03420666666667</v>
+        <v>19.878220321960455</v>
       </c>
       <c r="E26">
-        <v>34588404.750375479</v>
+        <v>34545578.366063245</v>
       </c>
       <c r="F26">
         <v>-2.2770281800000003</v>
@@ -4440,13 +4440,13 @@
         <v>0.02</v>
       </c>
       <c r="K26">
-        <v>22.413232984616016</v>
+        <v>27.073170813618695</v>
       </c>
       <c r="L26">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9246054845331286E-4</v>
       </c>
       <c r="M26">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -4457,13 +4457,13 @@
         <v>3.1518160000000002</v>
       </c>
       <c r="C27">
-        <v>17.960127659574468</v>
+        <v>17.959917069799591</v>
       </c>
       <c r="D27">
-        <v>30.399883333333342</v>
+        <v>29.662440816092278</v>
       </c>
       <c r="E27">
-        <v>40908724.981261969</v>
+        <v>40901610.334454075</v>
       </c>
       <c r="F27">
         <v>-2.2770281800000003</v>
@@ -4481,13 +4481,13 @@
         <v>0.02</v>
       </c>
       <c r="K27">
-        <v>20.380840809428314</v>
+        <v>25.455554333802819</v>
       </c>
       <c r="L27">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9176751129588768E-4</v>
       </c>
       <c r="M27">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -4498,13 +4498,13 @@
         <v>2.9042742000000001</v>
       </c>
       <c r="C28">
-        <v>17.11422340425532</v>
+        <v>17.114507469034077</v>
       </c>
       <c r="D28">
-        <v>26.49147</v>
+        <v>26.297856466469625</v>
       </c>
       <c r="E28">
-        <v>47011844.03641478</v>
+        <v>47048111.812928371</v>
       </c>
       <c r="F28">
         <v>-2.2770281800000003</v>
@@ -4522,13 +4522,13 @@
         <v>0.02</v>
       </c>
       <c r="K28">
-        <v>22.724505547699572</v>
+        <v>26.181602592258198</v>
       </c>
       <c r="L28">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9209343659594766E-4</v>
       </c>
       <c r="M28">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -4539,13 +4539,13 @@
         <v>2.6790431999999997</v>
       </c>
       <c r="C29">
-        <v>17.82458510638298</v>
+        <v>17.824453777045349</v>
       </c>
       <c r="D29">
-        <v>29.144753333333327</v>
+        <v>28.581953571121126</v>
       </c>
       <c r="E29">
-        <v>40218929.070819512</v>
+        <v>40207461.43728327</v>
       </c>
       <c r="F29">
         <v>-2.2770281800000003</v>
@@ -4563,13 +4563,13 @@
         <v>0.02</v>
       </c>
       <c r="K29">
-        <v>20.300906380552107</v>
+        <v>24.484051683566118</v>
       </c>
       <c r="L29">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.9164092053850667E-4</v>
       </c>
       <c r="M29">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -4580,13 +4580,13 @@
         <v>3.0122383999999993</v>
       </c>
       <c r="C30">
-        <v>17.925500000000003</v>
+        <v>17.925309659241936</v>
       </c>
       <c r="D30">
-        <v>25.243023333333333</v>
+        <v>25.223122614709169</v>
       </c>
       <c r="E30">
-        <v>48649579.672587067</v>
+        <v>48698979.050368257</v>
       </c>
       <c r="F30">
         <v>-2.2770281800000003</v>
@@ -4604,13 +4604,13 @@
         <v>0.02</v>
       </c>
       <c r="K30">
-        <v>19.86215245405662</v>
+        <v>22.347746848378549</v>
       </c>
       <c r="L30">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.919628571300044E-4</v>
       </c>
       <c r="M30">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -4621,13 +4621,13 @@
         <v>2.8544415999999999</v>
       </c>
       <c r="C31">
-        <v>17.988819148936173</v>
+        <v>17.988591781404498</v>
       </c>
       <c r="D31">
-        <v>23.81145333333334</v>
+        <v>23.990745788975296</v>
       </c>
       <c r="E31">
-        <v>40276519.829833947</v>
+        <v>40265411.353068456</v>
       </c>
       <c r="F31">
         <v>-2.2770281800000003</v>
@@ -4645,13 +4645,13 @@
         <v>0.02</v>
       </c>
       <c r="K31">
-        <v>21.650710440865563</v>
+        <v>21.999999999999922</v>
       </c>
       <c r="L31">
-        <v>-2.7397260273972606E-4</v>
+        <v>-1.912245780398832E-4</v>
       </c>
       <c r="M31">
-        <v>1</v>
+        <v>0.66999999999999993</v>
       </c>
     </row>
   </sheetData>
@@ -4666,8 +4666,8 @@
   </sheetPr>
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4751,10 +4751,10 @@
         <v>32</v>
       </c>
       <c r="L2">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1917808219178083E-4</v>
       </c>
       <c r="M2">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -4765,13 +4765,13 @@
         <v>5.3096127999999991</v>
       </c>
       <c r="C3">
-        <v>23.833478723404255</v>
+        <v>23.831003136462709</v>
       </c>
       <c r="D3">
-        <v>59.723530000000011</v>
+        <v>59.080197423168535</v>
       </c>
       <c r="E3">
-        <v>65253262.46974574</v>
+        <v>65213752.081050105</v>
       </c>
       <c r="F3">
         <v>2.7229718199999997</v>
@@ -4789,13 +4789,13 @@
         <v>0.06</v>
       </c>
       <c r="K3">
-        <v>33.607576099179624</v>
+        <v>33.609118809935438</v>
       </c>
       <c r="L3">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1921385198751792E-4</v>
       </c>
       <c r="M3">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -4806,13 +4806,13 @@
         <v>5.0646572000000001</v>
       </c>
       <c r="C4">
-        <v>19.451595744680855</v>
+        <v>19.451682526181493</v>
       </c>
       <c r="D4">
-        <v>49.933783333333331</v>
+        <v>50.652627048121893</v>
       </c>
       <c r="E4">
-        <v>75729721.580058306</v>
+        <v>75756149.407834798</v>
       </c>
       <c r="F4">
         <v>2.7229718199999997</v>
@@ -4830,13 +4830,13 @@
         <v>0.06</v>
       </c>
       <c r="K4">
-        <v>29.54131524310209</v>
+        <v>31.151976763793332</v>
       </c>
       <c r="L4">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1915210982148995E-4</v>
       </c>
       <c r="M4">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -4847,13 +4847,13 @@
         <v>4.7905199999999999</v>
       </c>
       <c r="C5">
-        <v>18.635372340425533</v>
+        <v>18.635936420179682</v>
       </c>
       <c r="D5">
-        <v>47.309906666666663</v>
+        <v>48.393844873597523</v>
       </c>
       <c r="E5">
-        <v>71227142.019598544</v>
+        <v>71222074.430716485</v>
       </c>
       <c r="F5">
         <v>2.7229718199999997</v>
@@ -4871,13 +4871,13 @@
         <v>0.06</v>
       </c>
       <c r="K5">
-        <v>33.024469038333471</v>
+        <v>32.177988512882614</v>
       </c>
       <c r="L5">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1881689886490616E-4</v>
       </c>
       <c r="M5">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -4888,13 +4888,13 @@
         <v>5.0649659999999992</v>
       </c>
       <c r="C6">
-        <v>17.749893617021275</v>
+        <v>17.750975493062569</v>
       </c>
       <c r="D6">
-        <v>42.321466666666666</v>
+        <v>44.099512181124283</v>
       </c>
       <c r="E6">
-        <v>83931684.388262674</v>
+        <v>84027739.442451</v>
       </c>
       <c r="F6">
         <v>2.7229718199999997</v>
@@ -4912,13 +4912,13 @@
         <v>0.06</v>
       </c>
       <c r="K6">
-        <v>32.016188586205516</v>
+        <v>32.195719809843951</v>
       </c>
       <c r="L6">
-        <v>1.3698630136986303E-4</v>
+        <v>2.189950229153288E-4</v>
       </c>
       <c r="M6">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -4929,13 +4929,13 @@
         <v>4.1198835999999996</v>
       </c>
       <c r="C7">
-        <v>17.63809574468085</v>
+        <v>17.639242996119293</v>
       </c>
       <c r="D7">
-        <v>52.557659999999998</v>
+        <v>52.911409222646277</v>
       </c>
       <c r="E7">
-        <v>74935719.387350217</v>
+        <v>74956247.252966791</v>
       </c>
       <c r="F7">
         <v>2.7229718199999997</v>
@@ -4953,13 +4953,13 @@
         <v>0.06</v>
       </c>
       <c r="K7">
-        <v>32.53978285409724</v>
+        <v>32.73704537469699</v>
       </c>
       <c r="L7">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1913762596753193E-4</v>
       </c>
       <c r="M7">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -4970,13 +4970,13 @@
         <v>4.3586245999999997</v>
       </c>
       <c r="C8">
-        <v>20.282659574468088</v>
+        <v>20.282260379565152</v>
       </c>
       <c r="D8">
-        <v>48.754843333333334</v>
+        <v>49.637728485752817</v>
       </c>
       <c r="E8">
-        <v>61504468.031064555</v>
+        <v>61447613.814878158</v>
       </c>
       <c r="F8">
         <v>2.7229718199999997</v>
@@ -4994,13 +4994,13 @@
         <v>0.06</v>
       </c>
       <c r="K8">
-        <v>33.023441888356132</v>
+        <v>33.762029973808936</v>
       </c>
       <c r="L8">
-        <v>1.3698630136986303E-4</v>
+        <v>2.187710638955208E-4</v>
       </c>
       <c r="M8">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -5011,13 +5011,13 @@
         <v>5.1722353999999999</v>
       </c>
       <c r="C9">
-        <v>18.811478723404257</v>
+        <v>18.811939822444316</v>
       </c>
       <c r="D9">
-        <v>52.981383333333333</v>
+        <v>53.276174352205231</v>
       </c>
       <c r="E9">
-        <v>72661475.034356385</v>
+        <v>72665923.677030087</v>
       </c>
       <c r="F9">
         <v>2.7229718199999997</v>
@@ -5035,13 +5035,13 @@
         <v>0.06</v>
       </c>
       <c r="K9">
-        <v>31.244673900752687</v>
+        <v>33.008246585317437</v>
       </c>
       <c r="L9">
-        <v>1.3698630136986303E-4</v>
+        <v>2.192619852187696E-4</v>
       </c>
       <c r="M9">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -5052,13 +5052,13 @@
         <v>5.4410458000000004</v>
       </c>
       <c r="C10">
-        <v>19.827553191489365</v>
+        <v>19.827420126521716</v>
       </c>
       <c r="D10">
-        <v>45.282183333333336</v>
+        <v>46.648265373468391</v>
       </c>
       <c r="E10">
-        <v>78833159.012392625</v>
+        <v>78884069.694421679</v>
       </c>
       <c r="F10">
         <v>2.7229718199999997</v>
@@ -5076,13 +5076,13 @@
         <v>0.06</v>
       </c>
       <c r="K10">
-        <v>31.275070474464282</v>
+        <v>32.284859770537537</v>
       </c>
       <c r="L10">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1989026599010219E-4</v>
       </c>
       <c r="M10">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -5093,13 +5093,13 @@
         <v>4.9061655999999996</v>
       </c>
       <c r="C11">
-        <v>20.647734042553196</v>
+        <v>20.647121365158686</v>
       </c>
       <c r="D11">
-        <v>64.308296666666678</v>
+        <v>63.027025165714946</v>
       </c>
       <c r="E11">
-        <v>66158734.32512299</v>
+        <v>66123906.544125788</v>
       </c>
       <c r="F11">
         <v>2.7229718199999997</v>
@@ -5117,13 +5117,13 @@
         <v>0.06</v>
       </c>
       <c r="K11">
-        <v>30.553750740657712</v>
+        <v>30.840153221951056</v>
       </c>
       <c r="L11">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1860709524022654E-4</v>
       </c>
       <c r="M11">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -5134,13 +5134,13 @@
         <v>4.2148395999999995</v>
       </c>
       <c r="C12">
-        <v>18.505765957446808</v>
+        <v>18.506405826378181</v>
       </c>
       <c r="D12">
-        <v>55.611943333333329</v>
+        <v>55.540709919940312</v>
       </c>
       <c r="E12">
-        <v>70131761.442441046</v>
+        <v>70119751.680564225</v>
       </c>
       <c r="F12">
         <v>2.7229718199999997</v>
@@ -5158,13 +5158,13 @@
         <v>0.06</v>
       </c>
       <c r="K12">
-        <v>35.219874752548762</v>
+        <v>34.061570685255624</v>
       </c>
       <c r="L12">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1918294485503498E-4</v>
       </c>
       <c r="M12">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -5175,13 +5175,13 @@
         <v>5.2603591999999999</v>
       </c>
       <c r="C13">
-        <v>19.898787234042555</v>
+        <v>19.898612513954603</v>
       </c>
       <c r="D13">
-        <v>57.274756666666669</v>
+        <v>56.972154150764737</v>
       </c>
       <c r="E13">
-        <v>77857618.443228394</v>
+        <v>77900588.962713003</v>
       </c>
       <c r="F13">
         <v>2.7229718199999997</v>
@@ -5199,13 +5199,13 @@
         <v>0.06</v>
       </c>
       <c r="K13">
-        <v>30.667352681930989</v>
+        <v>32.730466077942424</v>
       </c>
       <c r="L13">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1927447892771849E-4</v>
       </c>
       <c r="M13">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -5216,13 +5216,13 @@
         <v>4.4831096000000006</v>
       </c>
       <c r="C14">
-        <v>21.128563829787236</v>
+        <v>21.127669980330658</v>
       </c>
       <c r="D14">
-        <v>56.409933333333335</v>
+        <v>56.227665069298979</v>
       </c>
       <c r="E14">
-        <v>63876377.226617485</v>
+        <v>63830114.385199897</v>
       </c>
       <c r="F14">
         <v>2.7229718199999997</v>
@@ -5240,13 +5240,13 @@
         <v>0.06</v>
       </c>
       <c r="K14">
-        <v>33.922973981461439</v>
+        <v>34.654982770159677</v>
       </c>
       <c r="L14">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1884855148584864E-4</v>
       </c>
       <c r="M14">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -5257,13 +5257,13 @@
         <v>4.8162275999999995</v>
       </c>
       <c r="C15">
-        <v>19.724659574468085</v>
+        <v>19.724586678007551</v>
       </c>
       <c r="D15">
-        <v>60.946580000000004</v>
+        <v>60.13306838072829</v>
       </c>
       <c r="E15">
-        <v>78759734.914839268</v>
+        <v>78810040.186260134</v>
       </c>
       <c r="F15">
         <v>2.7229718199999997</v>
@@ -5281,13 +5281,13 @@
         <v>0.06</v>
       </c>
       <c r="K15">
-        <v>30.427216508733487</v>
+        <v>33.083741989648978</v>
       </c>
       <c r="L15">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1910147127354336E-4</v>
       </c>
       <c r="M15">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -5298,13 +5298,13 @@
         <v>4.7919868000000001</v>
       </c>
       <c r="C16">
-        <v>18.865893617021278</v>
+        <v>18.866322896177767</v>
       </c>
       <c r="D16">
-        <v>60.544243333333334</v>
+        <v>59.786714109443601</v>
       </c>
       <c r="E16">
-        <v>70309410.472354442</v>
+        <v>70298507.462686568</v>
       </c>
       <c r="F16">
         <v>2.7229718199999997</v>
@@ -5322,13 +5322,13 @@
         <v>0.06</v>
       </c>
       <c r="K16">
-        <v>33.708691527891908</v>
+        <v>34.7939762282967</v>
       </c>
       <c r="L16">
-        <v>1.3698630136986303E-4</v>
+        <v>2.2045133793531291E-4</v>
       </c>
       <c r="M16">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -5339,13 +5339,13 @@
         <v>5.1261083999999997</v>
       </c>
       <c r="C17">
-        <v>19.720702127659575</v>
+        <v>19.720631545372392</v>
       </c>
       <c r="D17">
-        <v>56.399239999999999</v>
+        <v>56.218459640161846</v>
       </c>
       <c r="E17">
-        <v>75635255.155803114</v>
+        <v>75660973.267977163</v>
       </c>
       <c r="F17">
         <v>2.7229718199999997</v>
@@ -5363,13 +5363,13 @@
         <v>0.06</v>
       </c>
       <c r="K17">
-        <v>33.806427779429328</v>
+        <v>36.601946718481841</v>
       </c>
       <c r="L17">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1890385307182423E-4</v>
       </c>
       <c r="M17">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -5380,13 +5380,13 @@
         <v>5.1965148000000001</v>
       </c>
       <c r="C18">
-        <v>19.197329787234043</v>
+        <v>19.197565254372442</v>
       </c>
       <c r="D18">
-        <v>48.956679999999999</v>
+        <v>49.811480960716231</v>
       </c>
       <c r="E18">
-        <v>74090464.547677249</v>
+        <v>74104874.446085662</v>
       </c>
       <c r="F18">
         <v>2.7229718199999997</v>
@@ -5404,13 +5404,13 @@
         <v>0.06</v>
       </c>
       <c r="K18">
-        <v>30.874099994381854</v>
+        <v>35.477589423619506</v>
       </c>
       <c r="L18">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1912319496117665E-4</v>
       </c>
       <c r="M18">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -5421,13 +5421,13 @@
         <v>4.1945745999999993</v>
       </c>
       <c r="C19">
-        <v>18.73826595744681</v>
+        <v>18.738769868693851</v>
       </c>
       <c r="D19">
-        <v>52.235523333333333</v>
+        <v>52.634095669890101</v>
       </c>
       <c r="E19">
-        <v>73973958.536680579</v>
+        <v>73987538.328484952</v>
       </c>
       <c r="F19">
         <v>2.7229718199999997</v>
@@ -5445,13 +5445,13 @@
         <v>0.06</v>
       </c>
       <c r="K19">
-        <v>30.96803159125562</v>
+        <v>34.447163725630936</v>
       </c>
       <c r="L19">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1898921673672408E-4</v>
       </c>
       <c r="M19">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -5462,13 +5462,13 @@
         <v>4.8746679999999998</v>
       </c>
       <c r="C20">
-        <v>20.362797872340426</v>
+        <v>20.362351815427147</v>
       </c>
       <c r="D20">
-        <v>55.134753333333329</v>
+        <v>55.129917644695688</v>
       </c>
       <c r="E20">
-        <v>73476815.423477843</v>
+        <v>73486888.904046863</v>
       </c>
       <c r="F20">
         <v>2.7229718199999997</v>
@@ -5486,13 +5486,13 @@
         <v>0.06</v>
       </c>
       <c r="K20">
-        <v>32.760822339220937</v>
+        <v>35.20952877560768</v>
       </c>
       <c r="L20">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1937535081983413E-4</v>
       </c>
       <c r="M20">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -5503,13 +5503,13 @@
         <v>5.0277555999999999</v>
       </c>
       <c r="C21">
-        <v>18.99154255319149</v>
+        <v>18.991898357344112</v>
       </c>
       <c r="D21">
-        <v>53.94645666666667</v>
+        <v>54.10696433183162</v>
       </c>
       <c r="E21">
-        <v>76722341.403616309</v>
+        <v>76756353.53431423</v>
       </c>
       <c r="F21">
         <v>2.7229718199999997</v>
@@ -5527,13 +5527,13 @@
         <v>0.06</v>
       </c>
       <c r="K21">
-        <v>33.324987783865851</v>
+        <v>36.536059270229337</v>
       </c>
       <c r="L21">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1926858360199762E-4</v>
       </c>
       <c r="M21">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -5544,13 +5544,13 @@
         <v>5.1486121999999996</v>
       </c>
       <c r="C22">
-        <v>18.683851063829788</v>
+        <v>18.6843867949604</v>
       </c>
       <c r="D22">
-        <v>53.986556666666672</v>
+        <v>54.141484691095869</v>
       </c>
       <c r="E22">
-        <v>69889349.176932305</v>
+        <v>69875841.135166764</v>
       </c>
       <c r="F22">
         <v>2.7229718199999997</v>
@@ -5568,13 +5568,13 @@
         <v>0.06</v>
       </c>
       <c r="K22">
-        <v>31.00126962170955</v>
+        <v>35.538871602694698</v>
       </c>
       <c r="L22">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1981347279091673E-4</v>
       </c>
       <c r="M22">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -5585,13 +5585,13 @@
         <v>5.2841367999999997</v>
       </c>
       <c r="C23">
-        <v>19.819638297872341</v>
+        <v>19.819509861251397</v>
       </c>
       <c r="D23">
-        <v>59.937396666666672</v>
+        <v>59.264306005911223</v>
       </c>
       <c r="E23">
-        <v>73109563.745479733</v>
+        <v>73117084.317750484</v>
       </c>
       <c r="F23">
         <v>2.7229718199999997</v>
@@ -5609,13 +5609,13 @@
         <v>0.06</v>
       </c>
       <c r="K23">
-        <v>33.787759486519995</v>
+        <v>37.3281737999705</v>
       </c>
       <c r="L23">
-        <v>1.3698630136986303E-4</v>
+        <v>2.199629634204734E-4</v>
       </c>
       <c r="M23">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -5626,13 +5626,13 @@
         <v>4.5869435999999997</v>
       </c>
       <c r="C24">
-        <v>19.007372340425533</v>
+        <v>19.007718887884749</v>
       </c>
       <c r="D24">
-        <v>68.580283333333341</v>
+        <v>66.704594106000172</v>
       </c>
       <c r="E24">
-        <v>70718988.906000718</v>
+        <v>70710665.787983701</v>
       </c>
       <c r="F24">
         <v>2.7229718199999997</v>
@@ -5650,13 +5650,13 @@
         <v>0.06</v>
       </c>
       <c r="K24">
-        <v>33.10740806318168</v>
+        <v>38.437124573908001</v>
       </c>
       <c r="L24">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1859015634857515E-4</v>
       </c>
       <c r="M24">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -5667,13 +5667,13 @@
         <v>4.6476228000000006</v>
       </c>
       <c r="C25">
-        <v>20.614095744680849</v>
+        <v>20.61350273775982</v>
       </c>
       <c r="D25">
-        <v>60.637810000000009</v>
+        <v>59.867261614393534</v>
       </c>
       <c r="E25">
-        <v>70675346.934262186</v>
+        <v>70666747.046057388</v>
       </c>
       <c r="F25">
         <v>2.7229718199999997</v>
@@ -5691,13 +5691,13 @@
         <v>0.06</v>
       </c>
       <c r="K25">
-        <v>30.219727833583054</v>
+        <v>36.658395118246865</v>
       </c>
       <c r="L25">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1909543690578153E-4</v>
       </c>
       <c r="M25">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -5708,13 +5708,13 @@
         <v>4.4569773999999995</v>
       </c>
       <c r="C26">
-        <v>19.447638297872341</v>
+        <v>19.44772739354633</v>
       </c>
       <c r="D26">
-        <v>49.03420666666667</v>
+        <v>49.878220321960455</v>
       </c>
       <c r="E26">
-        <v>64588404.750375479</v>
+        <v>64545578.366063245</v>
       </c>
       <c r="F26">
         <v>2.7229718199999997</v>
@@ -5732,13 +5732,13 @@
         <v>0.06</v>
       </c>
       <c r="K26">
-        <v>32.413232984616016</v>
+        <v>37.073170813618695</v>
       </c>
       <c r="L26">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1849835565627621E-4</v>
       </c>
       <c r="M26">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -5749,13 +5749,13 @@
         <v>5.1518160000000002</v>
       </c>
       <c r="C27">
-        <v>19.960127659574468</v>
+        <v>19.959917069799591</v>
       </c>
       <c r="D27">
-        <v>60.399883333333342</v>
+        <v>59.662440816092278</v>
       </c>
       <c r="E27">
-        <v>70908724.981261969</v>
+        <v>70901610.334454075</v>
       </c>
       <c r="F27">
         <v>2.7229718199999997</v>
@@ -5773,13 +5773,13 @@
         <v>0.06</v>
       </c>
       <c r="K27">
-        <v>30.380840809428314</v>
+        <v>35.455554333802823</v>
       </c>
       <c r="L27">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1919139281370142E-4</v>
       </c>
       <c r="M27">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -5790,13 +5790,13 @@
         <v>4.9042741999999997</v>
       </c>
       <c r="C28">
-        <v>19.11422340425532</v>
+        <v>19.114507469034077</v>
       </c>
       <c r="D28">
-        <v>56.49147</v>
+        <v>56.297856466469625</v>
       </c>
       <c r="E28">
-        <v>77011844.036414772</v>
+        <v>77048111.812928379</v>
       </c>
       <c r="F28">
         <v>2.7229718199999997</v>
@@ -5814,13 +5814,13 @@
         <v>0.06</v>
       </c>
       <c r="K28">
-        <v>32.724505547699572</v>
+        <v>36.181602592258201</v>
       </c>
       <c r="L28">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1886546751364143E-4</v>
       </c>
       <c r="M28">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -5831,13 +5831,13 @@
         <v>4.6790431999999997</v>
       </c>
       <c r="C29">
-        <v>19.82458510638298</v>
+        <v>19.824453777045349</v>
       </c>
       <c r="D29">
-        <v>59.144753333333327</v>
+        <v>58.581953571121126</v>
       </c>
       <c r="E29">
-        <v>70218929.070819512</v>
+        <v>70207461.437283278</v>
       </c>
       <c r="F29">
         <v>2.7229718199999997</v>
@@ -5855,13 +5855,13 @@
         <v>0.06</v>
       </c>
       <c r="K29">
-        <v>30.300906380552107</v>
+        <v>34.484051683566122</v>
       </c>
       <c r="L29">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1931798357108242E-4</v>
       </c>
       <c r="M29">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -5872,13 +5872,13 @@
         <v>5.0122383999999993</v>
       </c>
       <c r="C30">
-        <v>19.925500000000003</v>
+        <v>19.925309659241936</v>
       </c>
       <c r="D30">
-        <v>55.243023333333333</v>
+        <v>55.223122614709169</v>
       </c>
       <c r="E30">
-        <v>78649579.672587067</v>
+        <v>78698979.050368249</v>
       </c>
       <c r="F30">
         <v>2.7229718199999997</v>
@@ -5896,13 +5896,13 @@
         <v>0.06</v>
       </c>
       <c r="K30">
-        <v>29.86215245405662</v>
+        <v>32.347746848378549</v>
       </c>
       <c r="L30">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1899604697958469E-4</v>
       </c>
       <c r="M30">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -5913,13 +5913,13 @@
         <v>4.8544415999999995</v>
       </c>
       <c r="C31">
-        <v>19.988819148936173</v>
+        <v>19.988591781404498</v>
       </c>
       <c r="D31">
-        <v>53.81145333333334</v>
+        <v>53.990745788975296</v>
       </c>
       <c r="E31">
-        <v>70276519.829833955</v>
+        <v>70265411.353068456</v>
       </c>
       <c r="F31">
         <v>2.7229718199999997</v>
@@ -5937,13 +5937,13 @@
         <v>0.06</v>
       </c>
       <c r="K31">
-        <v>31.650710440865563</v>
+        <v>31.999999999999922</v>
       </c>
       <c r="L31">
-        <v>1.3698630136986303E-4</v>
+        <v>2.1973432606970587E-4</v>
       </c>
       <c r="M31">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix error in testing length/size of arrays
</commit_message>
<xml_diff>
--- a/ExcelInputs/GEPEP_calibration.xlsx
+++ b/ExcelInputs/GEPEP_calibration.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9717A61C-2AA2-4FF2-BBA5-2CE05AE7630C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B220D6BD-3F71-4A87-980E-0438CDD3DB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="699" activeTab="2" xr2:uid="{08305449-70BC-467B-94A3-5CFFCBC3DBD2}"/>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="3" xr2:uid="{81A49CF1-039D-452F-8A6F-A45C842E73DE}"/>
+    <workbookView xWindow="29610" yWindow="60" windowWidth="25140" windowHeight="15075" tabRatio="699" activeTab="2" xr2:uid="{08305449-70BC-467B-94A3-5CFFCBC3DBD2}"/>
+    <workbookView xWindow="29955" yWindow="405" windowWidth="25140" windowHeight="15075" activeTab="3" xr2:uid="{81A49CF1-039D-452F-8A6F-A45C842E73DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Weights" sheetId="10" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="coefficients">#REF!</definedName>
     <definedName name="HighAdj">#REF!</definedName>
     <definedName name="LowAdj">#REF!</definedName>
-    <definedName name="ProdnTargets">Targets!$B$3:$K$31</definedName>
+    <definedName name="ProdnTargets">Targets!$B$3:$J$31</definedName>
     <definedName name="Scenario">#REF!</definedName>
     <definedName name="StdCoeffs">#REF!</definedName>
     <definedName name="TeamNo">#REF!</definedName>
@@ -741,13 +741,14 @@
     <sheetView workbookViewId="0">
       <selection activeCell="O1" sqref="O1:P1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="K1" sqref="K1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
@@ -828,14 +829,13 @@
       <selection pane="bottomRight"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <selection activeCell="L3" sqref="L3:L31"/>
+      <selection activeCell="K1" sqref="K1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1850,7 +1850,7 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="K1" sqref="K1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,7 +1859,6 @@
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2874,9 +2873,7 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2884,7 +2881,6 @@
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3899,7 +3895,7 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="K1" sqref="K1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3908,7 +3904,6 @@
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Debugging the Cloud run
</commit_message>
<xml_diff>
--- a/ExcelInputs/GEPEP_calibration.xlsx
+++ b/ExcelInputs/GEPEP_calibration.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9262B3FE-7BFC-4A39-A720-DE2E02D4AB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C921FA7-294D-41EB-8E32-CCF284C6BADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="699" activeTab="2" xr2:uid="{08305449-70BC-467B-94A3-5CFFCBC3DBD2}"/>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="686" activeTab="2" xr2:uid="{81A49CF1-039D-452F-8A6F-A45C842E73DE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="686" activeTab="3" xr2:uid="{81A49CF1-039D-452F-8A6F-A45C842E73DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Weights" sheetId="10" r:id="rId1"/>
@@ -514,7 +514,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -543,6 +543,7 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -2097,7 +2098,7 @@
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView workbookViewId="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3315,11 +3316,11 @@
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView tabSelected="1" workbookViewId="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2:K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3396,13 +3397,13 @@
         <v>60</v>
       </c>
       <c r="I2" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J2" s="1">
         <v>18</v>
       </c>
-      <c r="K2" s="2">
-        <v>0</v>
+      <c r="K2" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L2" s="1">
         <v>0.64999999999999991</v>
@@ -3434,13 +3435,13 @@
         <v>62.903499999999994</v>
       </c>
       <c r="I3" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J3" s="1">
         <v>18.222280000000001</v>
       </c>
-      <c r="K3" s="2">
-        <v>0</v>
+      <c r="K3" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L3" s="1">
         <v>0.64999999999999991</v>
@@ -3472,13 +3473,13 @@
         <v>59.774000000000001</v>
       </c>
       <c r="I4" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J4" s="1">
         <v>16.851814999999998</v>
       </c>
-      <c r="K4" s="2">
-        <v>0</v>
+      <c r="K4" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L4" s="1">
         <v>0.64999999999999991</v>
@@ -3510,13 +3511,13 @@
         <v>60.713999999999999</v>
       </c>
       <c r="I5" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J5" s="1">
         <v>20.027245000000001</v>
       </c>
-      <c r="K5" s="2">
-        <v>0</v>
+      <c r="K5" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L5" s="1">
         <v>0.64999999999999991</v>
@@ -3548,13 +3549,13 @@
         <v>61.171500000000002</v>
       </c>
       <c r="I6" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J6" s="1">
         <v>16.625350000000001</v>
       </c>
-      <c r="K6" s="2">
-        <v>0</v>
+      <c r="K6" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L6" s="1">
         <v>0.64999999999999991</v>
@@ -3586,13 +3587,13 @@
         <v>58.521000000000001</v>
       </c>
       <c r="I7" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J7" s="1">
         <v>18.31371</v>
       </c>
-      <c r="K7" s="2">
-        <v>0</v>
+      <c r="K7" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L7" s="1">
         <v>0.64999999999999991</v>
@@ -3624,13 +3625,13 @@
         <v>59.145000000000003</v>
       </c>
       <c r="I8" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J8" s="1">
         <v>17.859439999999999</v>
       </c>
-      <c r="K8" s="2">
-        <v>0</v>
+      <c r="K8" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L8" s="1">
         <v>0.64999999999999991</v>
@@ -3662,13 +3663,13 @@
         <v>61.204500000000003</v>
       </c>
       <c r="I9" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J9" s="1">
         <v>19.298169999999999</v>
       </c>
-      <c r="K9" s="2">
-        <v>0</v>
+      <c r="K9" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L9" s="1">
         <v>0.64999999999999991</v>
@@ -3700,13 +3701,13 @@
         <v>63.600999999999999</v>
       </c>
       <c r="I10" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J10" s="1">
         <v>16.683199999999999</v>
       </c>
-      <c r="K10" s="2">
-        <v>0</v>
+      <c r="K10" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L10" s="1">
         <v>0.64999999999999991</v>
@@ -3738,13 +3739,13 @@
         <v>59.222999999999999</v>
       </c>
       <c r="I11" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J11" s="1">
         <v>21.160430000000002</v>
       </c>
-      <c r="K11" s="2">
-        <v>0</v>
+      <c r="K11" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L11" s="1">
         <v>0.64999999999999991</v>
@@ -3776,13 +3777,13 @@
         <v>60.963000000000008</v>
       </c>
       <c r="I12" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J12" s="1">
         <v>17.176154999999998</v>
       </c>
-      <c r="K12" s="2">
-        <v>0</v>
+      <c r="K12" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L12" s="1">
         <v>0.64999999999999991</v>
@@ -3814,13 +3815,13 @@
         <v>61.366500000000002</v>
       </c>
       <c r="I13" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J13" s="1">
         <v>18.691000000000003</v>
       </c>
-      <c r="K13" s="2">
-        <v>0</v>
+      <c r="K13" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L13" s="1">
         <v>0.64999999999999991</v>
@@ -3852,13 +3853,13 @@
         <v>58.55</v>
       </c>
       <c r="I14" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J14" s="1">
         <v>18.356735000000004</v>
       </c>
-      <c r="K14" s="2">
-        <v>0</v>
+      <c r="K14" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L14" s="1">
         <v>0.64999999999999991</v>
@@ -3890,13 +3891,13 @@
         <v>63.219000000000001</v>
       </c>
       <c r="I15" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J15" s="1">
         <v>18.368819999999996</v>
       </c>
-      <c r="K15" s="2">
-        <v>0</v>
+      <c r="K15" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L15" s="1">
         <v>0.64999999999999991</v>
@@ -3928,13 +3929,13 @@
         <v>57.028999999999996</v>
       </c>
       <c r="I16" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J16" s="1">
         <v>18.428129999999999</v>
       </c>
-      <c r="K16" s="2">
-        <v>0</v>
+      <c r="K16" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L16" s="1">
         <v>0.64999999999999991</v>
@@ -3966,13 +3967,13 @@
         <v>60.521000000000001</v>
       </c>
       <c r="I17" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J17" s="1">
         <v>17.072644999999998</v>
       </c>
-      <c r="K17" s="2">
-        <v>0</v>
+      <c r="K17" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L17" s="1">
         <v>0.64999999999999991</v>
@@ -4004,13 +4005,13 @@
         <v>59.486499999999999</v>
       </c>
       <c r="I18" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J18" s="1">
         <v>18.056084999999999</v>
       </c>
-      <c r="K18" s="2">
-        <v>0</v>
+      <c r="K18" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L18" s="1">
         <v>0.64999999999999991</v>
@@ -4042,13 +4043,13 @@
         <v>58.776000000000003</v>
       </c>
       <c r="I19" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J19" s="1">
         <v>17.597560000000001</v>
       </c>
-      <c r="K19" s="2">
-        <v>0</v>
+      <c r="K19" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L19" s="1">
         <v>0.64999999999999991</v>
@@ -4080,13 +4081,13 @@
         <v>62.811500000000009</v>
       </c>
       <c r="I20" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J20" s="1">
         <v>17.45271</v>
       </c>
-      <c r="K20" s="2">
-        <v>0</v>
+      <c r="K20" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L20" s="1">
         <v>0.64999999999999991</v>
@@ -4118,13 +4119,13 @@
         <v>60.568000000000005</v>
       </c>
       <c r="I21" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J21" s="1">
         <v>17.693754999999999</v>
       </c>
-      <c r="K21" s="2">
-        <v>0</v>
+      <c r="K21" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L21" s="1">
         <v>0.64999999999999991</v>
@@ -4156,13 +4157,13 @@
         <v>58.369</v>
       </c>
       <c r="I22" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J22" s="1">
         <v>18.655555000000003</v>
       </c>
-      <c r="K22" s="2">
-        <v>0</v>
+      <c r="K22" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L22" s="1">
         <v>0.64999999999999991</v>
@@ -4194,13 +4195,13 @@
         <v>59.688000000000002</v>
       </c>
       <c r="I23" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J23" s="1">
         <v>17.813374999999997</v>
       </c>
-      <c r="K23" s="2">
-        <v>0</v>
+      <c r="K23" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L23" s="1">
         <v>0.64999999999999991</v>
@@ -4232,13 +4233,13 @@
         <v>57.705500000000001</v>
       </c>
       <c r="I24" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J24" s="1">
         <v>18.578790000000001</v>
       </c>
-      <c r="K24" s="2">
-        <v>0</v>
+      <c r="K24" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L24" s="1">
         <v>0.64999999999999991</v>
@@ -4270,13 +4271,13 @@
         <v>58.845500000000001</v>
       </c>
       <c r="I25" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J25" s="1">
         <v>17.276835000000002</v>
       </c>
-      <c r="K25" s="2">
-        <v>0</v>
+      <c r="K25" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L25" s="1">
         <v>0.64999999999999991</v>
@@ -4308,13 +4309,13 @@
         <v>57.162999999999997</v>
       </c>
       <c r="I26" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J26" s="1">
         <v>17.838464999999999</v>
       </c>
-      <c r="K26" s="2">
-        <v>0</v>
+      <c r="K26" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L26" s="1">
         <v>0.64999999999999991</v>
@@ -4346,13 +4347,13 @@
         <v>60.446000000000005</v>
       </c>
       <c r="I27" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J27" s="1">
         <v>17.361775000000002</v>
       </c>
-      <c r="K27" s="2">
-        <v>0</v>
+      <c r="K27" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L27" s="1">
         <v>0.64999999999999991</v>
@@ -4384,13 +4385,13 @@
         <v>60.691499999999998</v>
       </c>
       <c r="I28" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J28" s="1">
         <v>17.831589999999998</v>
       </c>
-      <c r="K28" s="2">
-        <v>0</v>
+      <c r="K28" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L28" s="1">
         <v>0.64999999999999991</v>
@@ -4422,13 +4423,13 @@
         <v>59.313499999999998</v>
       </c>
       <c r="I29" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J29" s="1">
         <v>17.976212155999999</v>
       </c>
-      <c r="K29" s="2">
-        <v>0</v>
+      <c r="K29" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L29" s="1">
         <v>0.64999999999999991</v>
@@ -4460,13 +4461,13 @@
         <v>60.516500000000001</v>
       </c>
       <c r="I30" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J30" s="1">
         <v>17.058200000000003</v>
       </c>
-      <c r="K30" s="2">
-        <v>0</v>
+      <c r="K30" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L30" s="1">
         <v>0.64999999999999991</v>
@@ -4498,13 +4499,13 @@
         <v>57.713499999999996</v>
       </c>
       <c r="I31" s="1">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J31" s="1">
         <v>18.680225</v>
       </c>
-      <c r="K31" s="2">
-        <v>0</v>
+      <c r="K31" s="22">
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="L31" s="1">
         <v>0.64999999999999991</v>

</xml_diff>

<commit_message>
GEPEP calibration for iteration 1 of GFS for GSW Spring lambing
</commit_message>
<xml_diff>
--- a/ExcelInputs/GEPEP_calibration.xlsx
+++ b/ExcelInputs/GEPEP_calibration.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C921FA7-294D-41EB-8E32-CCF284C6BADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9262B3FE-7BFC-4A39-A720-DE2E02D4AB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="699" activeTab="2" xr2:uid="{08305449-70BC-467B-94A3-5CFFCBC3DBD2}"/>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="686" activeTab="3" xr2:uid="{81A49CF1-039D-452F-8A6F-A45C842E73DE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="686" activeTab="2" xr2:uid="{81A49CF1-039D-452F-8A6F-A45C842E73DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Weights" sheetId="10" r:id="rId1"/>
@@ -514,7 +514,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -543,7 +543,6 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -2098,7 +2097,7 @@
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView tabSelected="1" workbookViewId="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3316,11 +3315,11 @@
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView workbookViewId="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2:K31"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3397,13 +3396,13 @@
         <v>60</v>
       </c>
       <c r="I2" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J2" s="1">
         <v>18</v>
       </c>
-      <c r="K2" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K2" s="2">
+        <v>0</v>
       </c>
       <c r="L2" s="1">
         <v>0.64999999999999991</v>
@@ -3435,13 +3434,13 @@
         <v>62.903499999999994</v>
       </c>
       <c r="I3" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J3" s="1">
         <v>18.222280000000001</v>
       </c>
-      <c r="K3" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K3" s="2">
+        <v>0</v>
       </c>
       <c r="L3" s="1">
         <v>0.64999999999999991</v>
@@ -3473,13 +3472,13 @@
         <v>59.774000000000001</v>
       </c>
       <c r="I4" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J4" s="1">
         <v>16.851814999999998</v>
       </c>
-      <c r="K4" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K4" s="2">
+        <v>0</v>
       </c>
       <c r="L4" s="1">
         <v>0.64999999999999991</v>
@@ -3511,13 +3510,13 @@
         <v>60.713999999999999</v>
       </c>
       <c r="I5" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J5" s="1">
         <v>20.027245000000001</v>
       </c>
-      <c r="K5" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K5" s="2">
+        <v>0</v>
       </c>
       <c r="L5" s="1">
         <v>0.64999999999999991</v>
@@ -3549,13 +3548,13 @@
         <v>61.171500000000002</v>
       </c>
       <c r="I6" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J6" s="1">
         <v>16.625350000000001</v>
       </c>
-      <c r="K6" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K6" s="2">
+        <v>0</v>
       </c>
       <c r="L6" s="1">
         <v>0.64999999999999991</v>
@@ -3587,13 +3586,13 @@
         <v>58.521000000000001</v>
       </c>
       <c r="I7" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J7" s="1">
         <v>18.31371</v>
       </c>
-      <c r="K7" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K7" s="2">
+        <v>0</v>
       </c>
       <c r="L7" s="1">
         <v>0.64999999999999991</v>
@@ -3625,13 +3624,13 @@
         <v>59.145000000000003</v>
       </c>
       <c r="I8" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J8" s="1">
         <v>17.859439999999999</v>
       </c>
-      <c r="K8" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K8" s="2">
+        <v>0</v>
       </c>
       <c r="L8" s="1">
         <v>0.64999999999999991</v>
@@ -3663,13 +3662,13 @@
         <v>61.204500000000003</v>
       </c>
       <c r="I9" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J9" s="1">
         <v>19.298169999999999</v>
       </c>
-      <c r="K9" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K9" s="2">
+        <v>0</v>
       </c>
       <c r="L9" s="1">
         <v>0.64999999999999991</v>
@@ -3701,13 +3700,13 @@
         <v>63.600999999999999</v>
       </c>
       <c r="I10" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J10" s="1">
         <v>16.683199999999999</v>
       </c>
-      <c r="K10" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K10" s="2">
+        <v>0</v>
       </c>
       <c r="L10" s="1">
         <v>0.64999999999999991</v>
@@ -3739,13 +3738,13 @@
         <v>59.222999999999999</v>
       </c>
       <c r="I11" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J11" s="1">
         <v>21.160430000000002</v>
       </c>
-      <c r="K11" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K11" s="2">
+        <v>0</v>
       </c>
       <c r="L11" s="1">
         <v>0.64999999999999991</v>
@@ -3777,13 +3776,13 @@
         <v>60.963000000000008</v>
       </c>
       <c r="I12" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J12" s="1">
         <v>17.176154999999998</v>
       </c>
-      <c r="K12" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K12" s="2">
+        <v>0</v>
       </c>
       <c r="L12" s="1">
         <v>0.64999999999999991</v>
@@ -3815,13 +3814,13 @@
         <v>61.366500000000002</v>
       </c>
       <c r="I13" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J13" s="1">
         <v>18.691000000000003</v>
       </c>
-      <c r="K13" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K13" s="2">
+        <v>0</v>
       </c>
       <c r="L13" s="1">
         <v>0.64999999999999991</v>
@@ -3853,13 +3852,13 @@
         <v>58.55</v>
       </c>
       <c r="I14" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J14" s="1">
         <v>18.356735000000004</v>
       </c>
-      <c r="K14" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K14" s="2">
+        <v>0</v>
       </c>
       <c r="L14" s="1">
         <v>0.64999999999999991</v>
@@ -3891,13 +3890,13 @@
         <v>63.219000000000001</v>
       </c>
       <c r="I15" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J15" s="1">
         <v>18.368819999999996</v>
       </c>
-      <c r="K15" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K15" s="2">
+        <v>0</v>
       </c>
       <c r="L15" s="1">
         <v>0.64999999999999991</v>
@@ -3929,13 +3928,13 @@
         <v>57.028999999999996</v>
       </c>
       <c r="I16" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J16" s="1">
         <v>18.428129999999999</v>
       </c>
-      <c r="K16" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K16" s="2">
+        <v>0</v>
       </c>
       <c r="L16" s="1">
         <v>0.64999999999999991</v>
@@ -3967,13 +3966,13 @@
         <v>60.521000000000001</v>
       </c>
       <c r="I17" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J17" s="1">
         <v>17.072644999999998</v>
       </c>
-      <c r="K17" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K17" s="2">
+        <v>0</v>
       </c>
       <c r="L17" s="1">
         <v>0.64999999999999991</v>
@@ -4005,13 +4004,13 @@
         <v>59.486499999999999</v>
       </c>
       <c r="I18" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J18" s="1">
         <v>18.056084999999999</v>
       </c>
-      <c r="K18" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K18" s="2">
+        <v>0</v>
       </c>
       <c r="L18" s="1">
         <v>0.64999999999999991</v>
@@ -4043,13 +4042,13 @@
         <v>58.776000000000003</v>
       </c>
       <c r="I19" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J19" s="1">
         <v>17.597560000000001</v>
       </c>
-      <c r="K19" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K19" s="2">
+        <v>0</v>
       </c>
       <c r="L19" s="1">
         <v>0.64999999999999991</v>
@@ -4081,13 +4080,13 @@
         <v>62.811500000000009</v>
       </c>
       <c r="I20" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J20" s="1">
         <v>17.45271</v>
       </c>
-      <c r="K20" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K20" s="2">
+        <v>0</v>
       </c>
       <c r="L20" s="1">
         <v>0.64999999999999991</v>
@@ -4119,13 +4118,13 @@
         <v>60.568000000000005</v>
       </c>
       <c r="I21" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J21" s="1">
         <v>17.693754999999999</v>
       </c>
-      <c r="K21" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K21" s="2">
+        <v>0</v>
       </c>
       <c r="L21" s="1">
         <v>0.64999999999999991</v>
@@ -4157,13 +4156,13 @@
         <v>58.369</v>
       </c>
       <c r="I22" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J22" s="1">
         <v>18.655555000000003</v>
       </c>
-      <c r="K22" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K22" s="2">
+        <v>0</v>
       </c>
       <c r="L22" s="1">
         <v>0.64999999999999991</v>
@@ -4195,13 +4194,13 @@
         <v>59.688000000000002</v>
       </c>
       <c r="I23" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J23" s="1">
         <v>17.813374999999997</v>
       </c>
-      <c r="K23" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K23" s="2">
+        <v>0</v>
       </c>
       <c r="L23" s="1">
         <v>0.64999999999999991</v>
@@ -4233,13 +4232,13 @@
         <v>57.705500000000001</v>
       </c>
       <c r="I24" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J24" s="1">
         <v>18.578790000000001</v>
       </c>
-      <c r="K24" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K24" s="2">
+        <v>0</v>
       </c>
       <c r="L24" s="1">
         <v>0.64999999999999991</v>
@@ -4271,13 +4270,13 @@
         <v>58.845500000000001</v>
       </c>
       <c r="I25" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J25" s="1">
         <v>17.276835000000002</v>
       </c>
-      <c r="K25" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K25" s="2">
+        <v>0</v>
       </c>
       <c r="L25" s="1">
         <v>0.64999999999999991</v>
@@ -4309,13 +4308,13 @@
         <v>57.162999999999997</v>
       </c>
       <c r="I26" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J26" s="1">
         <v>17.838464999999999</v>
       </c>
-      <c r="K26" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K26" s="2">
+        <v>0</v>
       </c>
       <c r="L26" s="1">
         <v>0.64999999999999991</v>
@@ -4347,13 +4346,13 @@
         <v>60.446000000000005</v>
       </c>
       <c r="I27" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J27" s="1">
         <v>17.361775000000002</v>
       </c>
-      <c r="K27" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K27" s="2">
+        <v>0</v>
       </c>
       <c r="L27" s="1">
         <v>0.64999999999999991</v>
@@ -4385,13 +4384,13 @@
         <v>60.691499999999998</v>
       </c>
       <c r="I28" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J28" s="1">
         <v>17.831589999999998</v>
       </c>
-      <c r="K28" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K28" s="2">
+        <v>0</v>
       </c>
       <c r="L28" s="1">
         <v>0.64999999999999991</v>
@@ -4423,13 +4422,13 @@
         <v>59.313499999999998</v>
       </c>
       <c r="I29" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J29" s="1">
         <v>17.976212155999999</v>
       </c>
-      <c r="K29" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K29" s="2">
+        <v>0</v>
       </c>
       <c r="L29" s="1">
         <v>0.64999999999999991</v>
@@ -4461,13 +4460,13 @@
         <v>60.516500000000001</v>
       </c>
       <c r="I30" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J30" s="1">
         <v>17.058200000000003</v>
       </c>
-      <c r="K30" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K30" s="2">
+        <v>0</v>
       </c>
       <c r="L30" s="1">
         <v>0.64999999999999991</v>
@@ -4499,13 +4498,13 @@
         <v>57.713499999999996</v>
       </c>
       <c r="I31" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J31" s="1">
         <v>18.680225</v>
       </c>
-      <c r="K31" s="22">
-        <v>8.9999999999999999E-8</v>
+      <c r="K31" s="2">
+        <v>0</v>
       </c>
       <c r="L31" s="1">
         <v>0.64999999999999991</v>

</xml_diff>